<commit_message>
Update infill documentation and images
Removed outdated 'iso' infill images and updated 'top' infill images with new versions. Added new images for adaptive cubic and 2D honeycomb infill patterns. Updated strength_settings_infill.md to revise infill strength values, descriptions, and remove references to deleted images. Introduced documentation for 2D honeycomb infill and made minor corrections and clarifications throughout.
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE418122-33C2-4FFD-8794-9BE8F3BAC407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2002E5-7EEA-49F9-975D-35691E8EED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>Infill</t>
   </si>
@@ -104,12 +104,6 @@
     <t>min</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>T/tProm</t>
-  </si>
-  <si>
     <t>Material Usage</t>
   </si>
   <si>
@@ -122,15 +116,6 @@
     <t>Extra Low</t>
   </si>
   <si>
-    <t>Ultra Low</t>
-  </si>
-  <si>
-    <t>Ultra High</t>
-  </si>
-  <si>
-    <t>Extra High</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
   </si>
   <si>
     <t>g/t</t>
-  </si>
-  <si>
-    <t>g/T/prom</t>
   </si>
   <si>
     <t>100mm x 100mm x 100mm</t>
@@ -303,9 +285,6 @@
     <t>Material/Time</t>
   </si>
   <si>
-    <t>% Deviation</t>
-  </si>
-  <si>
     <t>2D Honeycomb</t>
   </si>
   <si>
@@ -344,12 +323,27 @@
   <si>
     <t>Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its Esthetic appeal and ability to fill space efficiently.
 Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for Esthetic purposes.</t>
+  </si>
+  <si>
+    <t>Max %</t>
+  </si>
+  <si>
+    <t>% Effective</t>
+  </si>
+  <si>
+    <t>g/t prom</t>
+  </si>
+  <si>
+    <t>t prom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -403,28 +397,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -464,6 +448,12 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -501,6 +491,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -525,6 +519,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -582,46 +582,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}" name="Infill" displayName="Infill" ref="D1:X24" totalsRowCount="1">
-  <autoFilter ref="D1:X23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}" name="Infill" displayName="Infill" ref="E1:Y23">
+  <autoFilter ref="E1:Y23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{3D89DC5A-8AB2-4952-BD08-8DD7EDC3072E}" name="Infill" totalsRowLabel="Total"/>
-    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="16" dataCellStyle="Porcentaje"/>
+    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="18" dataCellStyle="Porcentaje"/>
     <tableColumn id="21" xr3:uid="{85FC4B7C-12B9-4B99-B32D-798AC5127191}" name="Type"/>
-    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="17"/>
     <tableColumn id="17" xr3:uid="{94F205F5-D170-40A1-8C5F-879C636804AA}" name="X-Y Strength">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="16"/>
     <tableColumn id="16" xr3:uid="{D6A80A00-4E52-418C-9F58-C091734E73D4}" name="Z Strength">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="13" dataCellStyle="Porcentaje"/>
+    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="15" dataCellStyle="Porcentaje"/>
     <tableColumn id="5" xr3:uid="{CC2FB322-5D42-4375-BC4F-16927902366E}" name="hs"/>
     <tableColumn id="2" xr3:uid="{0B06FA91-5EDF-466A-8753-FFCA36B0EFB0}" name="min"/>
-    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Deviation" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="2" dataCellStyle="Porcentaje">
+    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Effective" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/(997.25*0.15)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{32CE485A-842B-45B3-8F5D-B93DF0C49C8F}" name="Material Usage" dataDxfId="11" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="T/tProm" dataDxfId="9" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="t prom" dataDxfId="8" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="8" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="7" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/T/prom" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/t prom" dataDxfId="4" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="6" dataCellStyle="Porcentaje"/>
-    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="5" dataCellStyle="Porcentaje">
+    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="3" dataCellStyle="Porcentaje"/>
+    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="2" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="Text" dataDxfId="4" dataCellStyle="Porcentaje">
+    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="Text" dataDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -631,7 +633,6 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -651,11 +652,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}" name="Rating" displayName="Rating" ref="A11:B20" totalsRowShown="0">
-  <autoFilter ref="A11:B20" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}" name="Rating" displayName="Rating" ref="A11:C20" totalsRowShown="0">
+  <autoFilter ref="A11:C20" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1D00CA6A-CEDD-45A1-8BA8-6DB7769D516C}" name="N"/>
-    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="1" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" xr3:uid="{18E14714-6899-4575-90B8-4F97863AF141}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -978,185 +980,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
         <v>96</v>
       </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="S1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="T1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2</v>
-      </c>
-      <c r="H2" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
         <v>8</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>13</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>158.77000000000001</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0613854767276678</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2">
+      <c r="Q2" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[% Effective]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R2">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>493</v>
       </c>
-      <c r="R2" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S2" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.94559721011333908</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="3">
+      <c r="T2" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="U2" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32204868154158217</v>
       </c>
-      <c r="U2" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V2" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1881012132687909</v>
       </c>
-      <c r="V2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="2" t="str">
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>concentric</v>
       </c>
-      <c r="X2" s="2" t="str">
+      <c r="Y2" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1166,97 +1171,97 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Concentric
 Fills the area with progressively smaller versions of the outer contour, creating a concentric pattern. Ideal for 100% infill or flexible prints.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-concentric](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-concentric.png?raw=true)
-![infill-iso-concentric](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-concentric.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
       <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-Low</v>
-      </c>
       <c r="I3">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3">
+      <c r="K3">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3">
         <v>8</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>7</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>148.6</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3">
+      <c r="Q3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>487</v>
       </c>
-      <c r="R3" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S3" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93408892763731477</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="3">
+      <c r="T3" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="U3" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30513347022587267</v>
       </c>
-      <c r="U3" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V3" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1256976567918875</v>
       </c>
-      <c r="V3" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="2" t="str">
+      <c r="W3" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[g/t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="X3" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>rectilinear</v>
       </c>
-      <c r="X3" s="2" t="str">
+      <c r="Y3" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1266,97 +1271,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Rectilinear
 Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding.
-- **Horizontal Strength (X-Y):** Normal-Low
-- **Vertical Strength (Z):** Low
+- **Horizontal Strength (X-Y):** 0,925
+- **Vertical Strength (Z):** 0,75
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal
-- **Material/Time (Higher better):** Normal
+- **Material/Time (Higher better):** Normal-High
 ![infill-top-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-rectilinear.png?raw=true)
-![infill-iso-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-rectilinear.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2">
         <v>0.15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I4">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J4">
         <v>6</v>
       </c>
-      <c r="J4" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4">
+      <c r="K4">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4">
         <v>8</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>148.87</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99520347622628891</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4">
+      <c r="Q4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>486</v>
       </c>
-      <c r="R4" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S4" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93217088055797737</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="U4" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30631687242798356</v>
       </c>
-      <c r="U4" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V4" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1300634613198943</v>
       </c>
-      <c r="V4" t="s">
-        <v>31</v>
-      </c>
-      <c r="W4" s="2" t="str">
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>grid</v>
       </c>
-      <c r="X4" s="2" t="str">
+      <c r="Y4" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1366,97 +1370,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Grid
 Two-layer pattern of perpendicular lines, forming a grid. Overlapping points may cause noise or artifacts.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-grid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-grid.png?raw=true)
-![infill-iso-grid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-grid.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
       <c r="F5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="H5" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-Low</v>
-      </c>
       <c r="I5">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5">
+      <c r="K5">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5">
         <v>8</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>4</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>148.54</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5">
+      <c r="Q5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>484</v>
       </c>
-      <c r="R5" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S5" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92833478639930256</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" s="3">
+      <c r="T5" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="U5" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30690082644628097</v>
       </c>
-      <c r="U5" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V5" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1322177830650146</v>
       </c>
-      <c r="V5" t="s">
-        <v>31</v>
-      </c>
-      <c r="W5" s="2" t="str">
+      <c r="W5" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-lattice</v>
       </c>
-      <c r="X5" s="2" t="str">
+      <c r="Y5" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1466,97 +1469,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Lattice
 Low-strength pattern with good flexibility. Angle 1 and angle 2 TBD.
-- **Horizontal Strength (X-Y):** Normal-Low
-- **Vertical Strength (Z):** Low
+- **Horizontal Strength (X-Y):** 0,925
+- **Vertical Strength (Z):** 0,75
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-2d-lattice](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-2d-lattice.png?raw=true)
-![infill-iso-2d-lattice](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-2d-lattice.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
       <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="H6" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I6">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
-      <c r="J6" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6">
+      <c r="K6">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6">
         <v>7</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>49</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>154.68</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0340436199548759</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6">
+      <c r="Q6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>469</v>
       </c>
-      <c r="R6" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S6" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.8995640802092415</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="T6" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U6" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.3298081023454158</v>
       </c>
-      <c r="U6" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V6" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.2167272496405854</v>
       </c>
-      <c r="V6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" s="2" t="str">
+      <c r="W6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>line</v>
       </c>
-      <c r="X6" s="2" t="str">
+      <c r="Y6" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1566,97 +1568,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Line
 Similar to [rectilinear](#rectilinear), but each line is slightly rotated to improve print speed.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Low
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 0,75
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-line](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-line.png?raw=true)
-![infill-iso-line](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-line.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
       <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7">
         <v>6</v>
       </c>
-      <c r="H7" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I7">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7">
+      <c r="K7">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7">
         <v>7</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>50</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>148.54</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7">
+      <c r="Q7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="R7" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S7" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="T7" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U7" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31604255319148933</v>
       </c>
-      <c r="U7" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V7" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1659434191563129</v>
       </c>
-      <c r="V7" t="s">
-        <v>33</v>
-      </c>
-      <c r="W7" s="2" t="str">
+      <c r="W7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X7" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cubic</v>
       </c>
-      <c r="X7" s="2" t="str">
+      <c r="Y7" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1666,97 +1667,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Cubic
 3D cube pattern with corners facing down, distributing force in all directions. Triangles in the horizontal plane provide good X-Y strength.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-cubic.png?raw=true)
-![infill-iso-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-cubic.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
       <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="H8" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I8">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="J8" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8">
+      <c r="K8">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>50</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>147.55000000000001</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9863792094927718</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8">
+      <c r="Q8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="R8" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S8" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="3">
+      <c r="T8" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U8" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31393617021276599</v>
       </c>
-      <c r="U8" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V8" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.158172556190346</v>
       </c>
-      <c r="V8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W8" s="2" t="str">
+      <c r="W8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X8" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>triangles</v>
       </c>
-      <c r="X8" s="2" t="str">
+      <c r="Y8" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1766,97 +1766,96 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Triangles
 Triangle-based grid, offering strong X-Y strength but with triple overlaps at intersections.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-triangles](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-triangles.png?raw=true)
-![infill-iso-triangles](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-triangles.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
-        <v>74</v>
-      </c>
       <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="H9" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I9">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="J9" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9">
+      <c r="K9">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9">
         <v>7</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>43</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>148.53</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99293055903735272</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9">
+      <c r="Q9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>463</v>
       </c>
-      <c r="R9" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S9" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.88805579773321708</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U9" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32079913606911448</v>
       </c>
-      <c r="U9" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V9" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1834913931485316</v>
       </c>
-      <c r="V9" t="s">
-        <v>33</v>
-      </c>
-      <c r="W9" s="2" t="str">
+      <c r="W9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tri-hexagon</v>
       </c>
-      <c r="X9" s="2" t="str">
+      <c r="Y9" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1866,91 +1865,90 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Tri-hexagon
 Similar to the [triangles](#triangles) pattern but offset to prevent triple overlaps at intersections. This design combines triangles and hexagons, providing excellent X-Y strength.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** Normal-High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,25
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-tri-hexagon](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-tri-hexagon.png?raw=true)
-![infill-iso-tri-hexagon](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-tri-hexagon.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>75</v>
-      </c>
       <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10">
         <v>6</v>
       </c>
-      <c r="H10" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I10">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J10">
         <v>6</v>
       </c>
-      <c r="J10" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10">
+      <c r="K10">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10">
         <v>10</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>49</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>141.77000000000001</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.94773961728085576</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10">
+      <c r="Q10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>649</v>
       </c>
-      <c r="R10" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S10" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2448125544899737</v>
       </c>
-      <c r="S10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T10" s="3">
+      <c r="T10" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="U10" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21844375963020032</v>
       </c>
-      <c r="U10" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V10" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.8058821871442029</v>
       </c>
-      <c r="V10" t="s">
-        <v>26</v>
-      </c>
-      <c r="W10" s="2" t="str">
+      <c r="W10" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>gyroid</v>
       </c>
-      <c r="X10" s="2" t="str">
+      <c r="Y10" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1960,97 +1958,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Gyroid
 Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** High
+- **Time:** Normal-High
 - **Material/Time (Higher better):** Low
 ![infill-top-gyroid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-gyroid.png?raw=true)
-![infill-iso-gyroid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-gyroid.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>76</v>
-      </c>
       <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
         <v>6</v>
       </c>
-      <c r="H11" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I11">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J11">
         <v>6</v>
       </c>
-      <c r="J11" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11">
+      <c r="K11">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11">
         <v>11</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>29</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>151.01</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0095094844154757</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11">
+      <c r="Q11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>689</v>
       </c>
-      <c r="R11" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S11" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.3215344376634699</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T11" s="3">
+      <c r="T11" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>High</v>
+      </c>
+      <c r="U11" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21917271407837444</v>
       </c>
-      <c r="U11" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V11" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.80857144412283</v>
       </c>
-      <c r="V11" t="s">
-        <v>26</v>
-      </c>
-      <c r="W11" s="2" t="str">
+      <c r="W11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tpms-d</v>
       </c>
-      <c r="X11" s="2" t="str">
+      <c r="Y11" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2060,97 +2060,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### TPMS-D
 Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** High
 - **Material/Time (Higher better):** Low
 ![infill-top-tpms-d](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-tpms-d.png?raw=true)
-![infill-iso-tpms-d](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-tpms-d.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>77</v>
-      </c>
       <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12">
         <v>6</v>
       </c>
-      <c r="H12" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I12">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J12">
         <v>6</v>
       </c>
-      <c r="J12" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12">
+      <c r="K12">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12">
         <v>17</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>36</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>190.54</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.2737695328820924</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q12">
+      <c r="Q12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>1056</v>
       </c>
-      <c r="R12" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S12" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>2.0254577157802962</v>
       </c>
-      <c r="S12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="3">
+      <c r="T12" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Ultra-High</v>
+      </c>
+      <c r="U12" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18043560606060605</v>
       </c>
-      <c r="U12" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V12" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.6656625993664127</v>
       </c>
-      <c r="V12" t="s">
-        <v>27</v>
-      </c>
-      <c r="W12" s="2" t="str">
+      <c r="W12" t="s">
+        <v>25</v>
+      </c>
+      <c r="X12" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>honeycomb</v>
       </c>
-      <c r="X12" s="2" t="str">
+      <c r="Y12" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2160,97 +2162,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Honeycomb
 Hexagonal pattern balancing strength and material use. Double walls in each hexagon increase material consumption.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** High
-- **Time:** Ultra High
+- **Time:** Ultra-High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-honeycomb.png?raw=true)
-![infill-iso-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-honeycomb.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13">
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="H13" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
       <c r="I13">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="J13">
         <v>5</v>
       </c>
-      <c r="J13" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13">
+      <c r="K13">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13">
         <v>5</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>29</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>97.57</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.65226038271914422</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q13">
+      <c r="Q13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R13">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>329</v>
       </c>
-      <c r="R13" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S13" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.63103748910200519</v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13" s="3">
+      <c r="T13" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Low</v>
+      </c>
+      <c r="U13" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29656534954407293</v>
       </c>
-      <c r="U13" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V13" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0940881667956823</v>
       </c>
-      <c r="V13" t="s">
-        <v>31</v>
-      </c>
-      <c r="W13" s="2" t="str">
+      <c r="W13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>adaptive-cubic</v>
       </c>
-      <c r="X13" s="2" t="str">
+      <c r="Y13" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2260,97 +2264,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Adaptive Cubic
 [Cubic](#cubic) pattern with adaptive density: denser near walls, sparser in the center. Saves material and time while maintaining strength, ideal for large prints.
-- **Horizontal Strength (X-Y):** Normal-High
-- **Vertical Strength (Z):** Normal-High
+- **Horizontal Strength (X-Y):** 1,25
+- **Vertical Strength (Z):** 1,25
 - **Density Calculation:** Cubic reduced in the center
 - **Material Usage:** Low
 - **Time:** Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-adaptive-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-adaptive-cubic.png?raw=true)
-![infill-iso-adaptive-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-adaptive-cubic.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14">
+        <v>73</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="H14" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-Low</v>
-      </c>
       <c r="I14">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J14">
         <v>4</v>
       </c>
-      <c r="J14" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14">
-        <v>8</v>
+      <c r="K14">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
       <c r="N14">
+        <v>8</v>
+      </c>
+      <c r="O14">
         <v>148.6</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14">
+      <c r="Q14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>488</v>
       </c>
-      <c r="R14" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S14" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93600697471665206</v>
       </c>
-      <c r="S14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T14" s="3">
+      <c r="T14" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal</v>
+      </c>
+      <c r="U14" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30450819672131146</v>
       </c>
-      <c r="U14" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V14" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1233908992984614</v>
       </c>
-      <c r="V14" t="s">
-        <v>31</v>
-      </c>
-      <c r="W14" s="2" t="str">
+      <c r="W14" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>aligned-rectilinear</v>
       </c>
-      <c r="X14" s="2" t="str">
+      <c r="Y14" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2360,98 +2366,100 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Aligned Rectilinear
 Parallel lines spaced by the infill spacing, each layer printed in the same direction as the previous layer. Good horizontal strength perpendicular to the lines, but terrible in parallel direction.
 Recommended with layer anchoring to improve not perpendicular strength.
-- **Horizontal Strength (X-Y):** Normal-Low
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 0,925
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
 - **Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-aligned-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-aligned-rectilinear.png?raw=true)
-![infill-iso-aligned-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-aligned-rectilinear.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>94</v>
+      <c r="B15" s="7">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="7">
+        <v>87</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="H15" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-Low</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="I15">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J15">
         <v>3</v>
       </c>
-      <c r="J15" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-Low</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15">
+      <c r="K15">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15">
         <v>8</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>2</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>147.52000000000001</v>
       </c>
-      <c r="O15" s="8">
+      <c r="P15" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.98617865797610094</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>482</v>
       </c>
-      <c r="R15" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S15" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92449869224062775</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" s="3">
+      <c r="T15" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U15" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30605809128630707</v>
       </c>
-      <c r="U15" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V15" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1291087665609367</v>
       </c>
-      <c r="V15" t="s">
-        <v>31</v>
-      </c>
-      <c r="W15" s="8" t="str">
+      <c r="W15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-honeycomb</v>
       </c>
-      <c r="X15" s="8" t="str">
+      <c r="Y15" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2461,97 +2469,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Honeycomb
 Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve interlayer point of contact and reduce the risk of delamination.
-- **Horizontal Strength (X-Y):** Normal-Low
-- **Vertical Strength (Z):** Normal-Low
+- **Horizontal Strength (X-Y):** 0,925
+- **Vertical Strength (Z):** 0,925
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-2d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-2d-honeycomb.png?raw=true)
-![infill-iso-2d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-2d-honeycomb.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="7">
+        <v>1.075</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
-        <v>80</v>
-      </c>
       <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16">
         <v>4</v>
       </c>
-      <c r="H16" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
       <c r="I16">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="J16">
         <v>5</v>
       </c>
-      <c r="J16" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16">
+      <c r="K16">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16">
         <v>12</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>28</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>123.92</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.82841146486170303</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q16">
+      <c r="Q16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>748</v>
       </c>
-      <c r="R16" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S16" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.4346992153443765</v>
       </c>
-      <c r="S16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T16" s="3">
+      <c r="T16" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>High</v>
+      </c>
+      <c r="U16" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16566844919786097</v>
       </c>
-      <c r="U16" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V16" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.61118364015697213</v>
       </c>
-      <c r="V16" t="s">
-        <v>27</v>
-      </c>
-      <c r="W16" s="2" t="str">
+      <c r="W16" t="s">
+        <v>25</v>
+      </c>
+      <c r="X16" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>3d-honeycomb</v>
       </c>
-      <c r="X16" s="2" t="str">
+      <c r="Y16" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2561,97 +2571,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 3D Honeycomb
 This infill tries to generate a printable honeycomb structure by printing squares and octagons mantaining a vertical angle high enough to mantian contact with the previous layer.
-- **Horizontal Strength (X-Y):** Normal
-- **Vertical Strength (Z):** Normal-High
+- **Horizontal Strength (X-Y):** 1,075
+- **Vertical Strength (Z):** 1,25
 - **Density Calculation:** Unknown
 - **Material Usage:** Normal-Low
 - **Time:** High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-3d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-3d-honeycomb.png?raw=true)
-![infill-iso-3d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-3d-honeycomb.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="165" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17">
+        <v>94</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="H17" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I17">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J17">
         <v>4</v>
       </c>
-      <c r="J17" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L17">
+      <c r="K17">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17">
         <v>13</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>24</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>148.63</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99359906409292209</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q17">
+      <c r="Q17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>804</v>
       </c>
-      <c r="R17" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S17" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.5421098517872711</v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T17" s="3">
+      <c r="T17" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>High</v>
+      </c>
+      <c r="U17" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18486318407960198</v>
       </c>
-      <c r="U17" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V17" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.68199680943375651</v>
       </c>
-      <c r="V17" t="s">
-        <v>27</v>
-      </c>
-      <c r="W17" s="2" t="str">
+      <c r="W17" t="s">
+        <v>25</v>
+      </c>
+      <c r="X17" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>hilbert-curve</v>
       </c>
-      <c r="X17" s="2" t="str">
+      <c r="Y17" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2661,98 +2673,100 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Hilbert Curve
 Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its Esthetic appeal and ability to fill space efficiently.
 Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for Esthetic purposes.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Extra High
+- **Time:** High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-hilbert-curve](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-hilbert-curve.png?raw=true)
-![infill-iso-hilbert-curve](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-hilbert-curve.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
       <c r="F18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G18">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18">
         <v>2</v>
       </c>
-      <c r="H18" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I18">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J18">
         <v>4</v>
       </c>
-      <c r="J18" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L18">
+      <c r="K18">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18">
         <v>7</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>46</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>148.21</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99079134285953041</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q18">
+      <c r="Q18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>466</v>
       </c>
-      <c r="R18" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S18" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.89380993897122929</v>
       </c>
-      <c r="S18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T18" s="3">
+      <c r="T18" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U18" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31804721030042921</v>
       </c>
-      <c r="U18" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V18" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1733389952906987</v>
       </c>
-      <c r="V18" t="s">
-        <v>33</v>
-      </c>
-      <c r="W18" s="2" t="str">
+      <c r="W18" t="s">
+        <v>28</v>
+      </c>
+      <c r="X18" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>archimedean-chords</v>
       </c>
-      <c r="X18" s="2" t="str">
+      <c r="Y18" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2762,97 +2776,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Archimedean Chords
 Spiral pattern that fills the area with concentric arcs, creating a smooth and continuous infill. Can be filled with resin thanks to its interconnected hollow structure, which allows the resin to flow through it and cure properly.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-archimedean-chords](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-archimedean-chords.png?raw=true)
-![infill-iso-archimedean-chords](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-archimedean-chords.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19">
+      <c r="H19">
         <v>2</v>
       </c>
-      <c r="H19" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I19">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J19">
         <v>4</v>
       </c>
-      <c r="J19" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19">
+      <c r="K19">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.075</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19">
         <v>9</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>30</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>148.72</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99420071864293469</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q19">
+      <c r="Q19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>570</v>
       </c>
-      <c r="R19" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S19" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.0932868352223191</v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T19" s="3">
+      <c r="T19" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="U19" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.26091228070175437</v>
       </c>
-      <c r="U19" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V19" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.96255695187019885</v>
       </c>
-      <c r="V19" t="s">
-        <v>31</v>
-      </c>
-      <c r="W19" s="2" t="str">
+      <c r="W19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X19" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>octagram-spiral</v>
       </c>
-      <c r="X19" s="2" t="str">
+      <c r="Y19" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2862,97 +2878,99 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Octagram Spiral
 Esthetic pattern with low strength and high print time.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Normal
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 1,075
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** High
+- **Time:** Normal-High
 - **Material/Time (Higher better):** Normal
 ![infill-top-octagram-spiral](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-octagram-spiral.png?raw=true)
-![infill-iso-octagram-spiral](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-octagram-spiral.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B20" s="7">
+        <v>9.99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
       <c r="F20" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20">
+        <v>76</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20">
         <v>2</v>
       </c>
-      <c r="H20" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I20">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J20">
         <v>2</v>
       </c>
-      <c r="J20" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20">
+      <c r="K20">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20">
         <v>2</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>50</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>49.39</v>
       </c>
-      <c r="O20" s="2">
+      <c r="P20" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.33017464694576754</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q20">
+      <c r="Q20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R20">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>170</v>
       </c>
-      <c r="R20" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S20" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.32606800348735832</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T20" s="3">
+      <c r="T20" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Extra-Low</v>
+      </c>
+      <c r="U20" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29052941176470587</v>
       </c>
-      <c r="U20" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V20" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0718203998091715</v>
       </c>
-      <c r="V20" t="s">
-        <v>31</v>
-      </c>
-      <c r="W20" s="2" t="str">
+      <c r="W20" t="s">
+        <v>26</v>
+      </c>
+      <c r="X20" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>support-cubic</v>
       </c>
-      <c r="X20" s="2" t="str">
+      <c r="Y20" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2962,91 +2980,90 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Support Cubic
 Support |Cubic is a variation of the [Cubic](#cubic) infill pattern that is specifically designed for support top layers. Will use more material than Lightning infill but will provide better strength. Nevertheless, it is still a low-density infill pattern.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Low
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 0,75
 - **Density Calculation:** before top shell layers
-- **Material Usage:** Extra Low
-- **Time:** Extra Low
+- **Material Usage:** Extra-Low
+- **Time:** Extra-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-support-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-support-cubic.png?raw=true)
-![infill-iso-support-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-support-cubic.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
       <c r="F21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21">
         <v>2</v>
       </c>
-      <c r="H21" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
       <c r="I21">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="J21">
         <v>2</v>
       </c>
-      <c r="J21" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Low</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21">
+      <c r="K21">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>0.75</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21">
         <v>1</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>16</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>12.33</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>8.2426673351717217E-2</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q21">
+      <c r="Q21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R21">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>76</v>
       </c>
-      <c r="R21" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S21" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.14577157802964255</v>
       </c>
-      <c r="S21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T21" s="3">
+      <c r="T21" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Ultra-Low</v>
+      </c>
+      <c r="U21" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16223684210526315</v>
       </c>
-      <c r="U21" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V21" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.59852376361078963</v>
       </c>
-      <c r="V21" t="s">
-        <v>27</v>
-      </c>
-      <c r="W21" s="2" t="str">
+      <c r="W21" t="s">
+        <v>25</v>
+      </c>
+      <c r="X21" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>lightning</v>
       </c>
-      <c r="X21" s="2" t="str">
+      <c r="Y21" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3056,91 +3073,90 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Lightning
 Ultra-fast, ultra-low material infill. Designed for speed and efficiency, ideal for quick prints or non-structural prototypes.
-- **Horizontal Strength (X-Y):** Low
-- **Vertical Strength (Z):** Low
+- **Horizontal Strength (X-Y):** 0,75
+- **Vertical Strength (Z):** 0,75
 - **Density Calculation:** before top shell layers
-- **Material Usage:** Ultra Low
-- **Time:** Ultra Low
+- **Material Usage:** Ultra-Low
+- **Time:** Ultra-Low
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-lightning](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-lightning.png?raw=true)
-![infill-iso-lightning](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-lightning.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
       <c r="F22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22">
+        <v>78</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22">
         <v>5</v>
       </c>
-      <c r="H22" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
       <c r="I22">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="J22">
         <v>5</v>
       </c>
-      <c r="J22" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>Normal-High</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22">
+      <c r="K22">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.25</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22">
         <v>10</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>40</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>144.69999999999999</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.96732681540904142</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q22">
+      <c r="Q22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R22">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>640</v>
       </c>
-      <c r="R22" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S22" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2275501307759371</v>
       </c>
-      <c r="S22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T22" s="3">
+      <c r="T22" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="U22" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.22609374999999998</v>
       </c>
-      <c r="U22" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V22" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.83410451302470801</v>
       </c>
-      <c r="V22" t="s">
-        <v>26</v>
-      </c>
-      <c r="W22" s="2" t="str">
+      <c r="W22" t="s">
+        <v>24</v>
+      </c>
+      <c r="X22" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cross-hatch</v>
       </c>
-      <c r="X22" s="2" t="str">
+      <c r="Y22" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3150,91 +3166,90 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Cross Hatch
 Similar to [Gyroid](#gyroid) but with linear patterns, creating weak points at internal corners.
-- **Horizontal Strength (X-Y):** Normal-High
-- **Vertical Strength (Z):** Normal-High
+- **Horizontal Strength (X-Y):** 1,25
+- **Vertical Strength (Z):** 1,25
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** High
+- **Time:** Normal-High
 - **Material/Time (Higher better):** Low
 ![infill-top-cross-hatch](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-cross-hatch.png?raw=true)
-![infill-iso-cross-hatch](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-cross-hatch.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23">
         <v>6</v>
       </c>
-      <c r="H23" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
       <c r="I23">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="J23">
         <v>6</v>
       </c>
-      <c r="J23" t="str">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
-        <v>High</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23">
+      <c r="K23">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
+        <v>1.6</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M23">
         <v>8</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>1</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>148.55000000000001</v>
       </c>
-      <c r="O23" s="2">
+      <c r="P23" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99306426004846671</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q23">
+      <c r="Q23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>481</v>
       </c>
-      <c r="R23" s="2">
-        <f>Infill[[#This Row],[Total Time]]/Infill[[#Totals],[Total Time]]</f>
+      <c r="S23" s="2">
+        <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92258064516129035</v>
       </c>
-      <c r="S23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T23" s="3">
+      <c r="T23" s="2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="U23" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30883575883575887</v>
       </c>
-      <c r="U23" s="2">
-        <f>Infill[[#This Row],[g/t]]/Infill[[#Totals],[g/t]]</f>
+      <c r="V23" s="2">
+        <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1393561309338132</v>
       </c>
-      <c r="V23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W23" s="2" t="str">
+      <c r="W23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X23" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>quarter-cubic</v>
       </c>
-      <c r="X23" s="2" t="str">
+      <c r="Y23" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3244,46 +3259,23 @@
 - **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
-![infill-iso-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Quarter Cubic
 [Cubic](#cubic) pattern with extra internal divisions, improving X-Y strength.
-- **Horizontal Strength (X-Y):** High
-- **Vertical Strength (Z):** High
+- **Horizontal Strength (X-Y):** 1,6
+- **Vertical Strength (Z):** 1,6
 - **Density Calculation:** Total infill material usage
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Time:** Normal-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-quarter-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-quarter-cubic.png?raw=true)
-![infill-iso-quarter-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-iso-quarter-cubic.png?raw=true)
 </v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="4">
-        <f>SUBTOTAL(101,Infill[g])</f>
-        <v>136.61545454545453</v>
-      </c>
-      <c r="O24" s="1">
-        <f>SUBTOTAL(101,Infill[% Deviation])</f>
-        <v>0.91328122032559211</v>
-      </c>
-      <c r="Q24" s="4">
-        <f>SUBTOTAL(101,Infill[Total Time])</f>
-        <v>521.36363636363637</v>
-      </c>
-      <c r="T24" s="4">
-        <f>SUBTOTAL(101,Infill[g/t])</f>
-        <v>0.27106165530757964</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="O2:O23">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="P2:P23">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3294,8 +3286,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R23">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="S2:S23">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3306,7 +3298,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T23">
+  <conditionalFormatting sqref="U2:U23">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3318,8 +3310,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U23">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="V2:V23">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Revise infill pattern documentation and add comparison table
Updated strength_settings_infill.md to clarify infill density calculation, add a comprehensive comparison table of infill patterns, and standardize terminology for strength and print time. Expanded pattern descriptions to use qualitative strength ratings instead of numeric values. Updated infill_desc_calculator.xlsx to reflect these changes.
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2002E5-7EEA-49F9-975D-35691E8EED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207EB570-29FA-4B00-968A-CB3FC33489BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>Infill</t>
   </si>
@@ -125,15 +125,9 @@
     <t>Normal-High</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>DensityCalc</t>
   </si>
   <si>
-    <t>before top shell layers</t>
-  </si>
-  <si>
     <t>X-Y Strength</t>
   </si>
   <si>
@@ -213,12 +207,6 @@
   </si>
   <si>
     <t>Infill Combination</t>
-  </si>
-  <si>
-    <t>Total infill material usage</t>
-  </si>
-  <si>
-    <t>Cubic reduced in the center</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -306,18 +294,6 @@
     <t>Low-strength pattern with good flexibility. Angle 1 and angle 2 TBD.</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>Adaptative</t>
-  </si>
-  <si>
-    <t>Esthetic</t>
-  </si>
-  <si>
     <t>Esthetic pattern with low strength and high print time.</t>
   </si>
   <si>
@@ -335,6 +311,21 @@
   </si>
   <si>
     <t>t prom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> % of  total infill volume</t>
+  </si>
+  <si>
+    <t>Same as [Cubic](#cubic) but reduced in the center</t>
+  </si>
+  <si>
+    <t>% of layer before top shell layers</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>MD</t>
   </si>
 </sst>
 </file>
@@ -387,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -398,14 +389,55 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -551,22 +583,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,51 +606,53 @@
   <autoFilter ref="E1:Y23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{3D89DC5A-8AB2-4952-BD08-8DD7EDC3072E}" name="Infill" totalsRowLabel="Total"/>
-    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="18" dataCellStyle="Porcentaje"/>
-    <tableColumn id="21" xr3:uid="{85FC4B7C-12B9-4B99-B32D-798AC5127191}" name="Type"/>
-    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{94F205F5-D170-40A1-8C5F-879C636804AA}" name="X-Y Strength">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</calculatedColumnFormula>
+    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="2" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="21"/>
+    <tableColumn id="17" xr3:uid="{94F205F5-D170-40A1-8C5F-879C636804AA}" name="X-Y Strength" dataDxfId="20">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{D6A80A00-4E52-418C-9F58-C091734E73D4}" name="Z Strength">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</calculatedColumnFormula>
+    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{D6A80A00-4E52-418C-9F58-C091734E73D4}" name="Z Strength" dataDxfId="18">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="15" dataCellStyle="Porcentaje"/>
+    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="17" dataCellStyle="Porcentaje"/>
     <tableColumn id="5" xr3:uid="{CC2FB322-5D42-4375-BC4F-16927902366E}" name="hs"/>
     <tableColumn id="2" xr3:uid="{0B06FA91-5EDF-466A-8753-FFCA36B0EFB0}" name="min"/>
-    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Effective" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Porcentaje">
+    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Effective" totalsRowFunction="average" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/(997.25*0.15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{32CE485A-842B-45B3-8F5D-B93DF0C49C8F}" name="Material Usage" dataDxfId="11" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="11" xr3:uid="{32CE485A-842B-45B3-8F5D-B93DF0C49C8F}" name="Material Usage" dataDxfId="13" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="t prom" dataDxfId="8" dataCellStyle="Porcentaje">
+    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="t prom" dataDxfId="10" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="7" dataCellStyle="Porcentaje">
+    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="9" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Porcentaje">
+    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/t prom" dataDxfId="4" dataCellStyle="Porcentaje">
+    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/t prom" dataDxfId="6" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="3" dataCellStyle="Porcentaje"/>
-    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="2" dataCellStyle="Porcentaje">
+    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="5" dataCellStyle="Porcentaje"/>
+    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="4" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="Text" dataDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="21" xr3:uid="{75AA760A-15C0-4692-B168-BF74BE6D50F6}" name="Ref" dataDxfId="1" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="MD" dataDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</calculatedColumnFormula>
@@ -656,7 +678,7 @@
   <autoFilter ref="A11:C20" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1D00CA6A-CEDD-45A1-8BA8-6DB7769D516C}" name="N"/>
-    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="1" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="3" dataCellStyle="Porcentaje"/>
     <tableColumn id="3" xr3:uid="{18E14714-6899-4575-90B8-4F97863AF141}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -982,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,174 +1014,162 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="31.140625" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="55.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="23" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" customWidth="1"/>
+    <col min="25" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="B2" t="s">
         <v>52</v>
-      </c>
-      <c r="S1" t="s">
-        <v>98</v>
-      </c>
-      <c r="T1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W1" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="5">
         <v>2</v>
       </c>
+      <c r="H2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I2">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J2">
         <v>4</v>
       </c>
-      <c r="K2">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>59</v>
+      <c r="J2" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
       </c>
       <c r="M2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N2">
-        <v>13</v>
-      </c>
-      <c r="O2">
         <v>158.77000000000001</v>
       </c>
-      <c r="P2" s="2">
+      <c r="O2" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0613854767276678</v>
       </c>
-      <c r="Q2" s="2" t="str">
+      <c r="P2" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[% Effective]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>493</v>
       </c>
-      <c r="S2" s="2">
+      <c r="R2" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.94559721011333908</v>
       </c>
-      <c r="T2" s="2" t="str">
+      <c r="S2" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="U2" s="3">
+      <c r="T2" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32204868154158217</v>
       </c>
-      <c r="V2" s="2">
+      <c r="U2" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1881012132687909</v>
       </c>
-      <c r="W2" t="s">
+      <c r="V2" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="2" t="str">
+      <c r="W2" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>concentric</v>
+      </c>
+      <c r="X2" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Concentric](#concentric)</v>
       </c>
       <c r="Y2" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1168,98 +1178,99 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Concentric
 Fills the area with progressively smaller versions of the outer contour, creating a concentric pattern. Ideal for 100% infill or flexible prints.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Print Time:** Normal
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-concentric](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-concentric.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3">
+      <c r="F3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
+      <c r="H3" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-Low</v>
+      </c>
       <c r="I3">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>59</v>
+      <c r="J3" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N3">
-        <v>7</v>
-      </c>
-      <c r="O3">
         <v>148.6</v>
       </c>
-      <c r="P3" s="2">
+      <c r="O3" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R3">
+      <c r="Q3">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>487</v>
       </c>
-      <c r="S3" s="2">
+      <c r="R3" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93408892763731477</v>
       </c>
-      <c r="T3" s="2" t="str">
+      <c r="S3" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="U3" s="3">
+      <c r="T3" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30513347022587267</v>
       </c>
-      <c r="V3" s="2">
+      <c r="U3" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1256976567918875</v>
       </c>
-      <c r="W3" t="str">
+      <c r="V3" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[g/t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="X3" s="2" t="str">
+      <c r="W3" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>rectilinear</v>
+      </c>
+      <c r="X3" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Rectilinear](#rectilinear)</v>
       </c>
       <c r="Y3" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1268,25 +1279,25 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Rectilinear
 Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding.
-- **Horizontal Strength (X-Y):** 0,925
-- **Vertical Strength (Z):** 0,75
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Normal-Low
+- **Vertical Strength (Z):** Low
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Print Time:** Normal
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-rectilinear.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2">
         <v>0.15</v>
@@ -1294,71 +1305,72 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4">
         <v>6</v>
       </c>
+      <c r="H4" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I4">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J4">
         <v>6</v>
       </c>
-      <c r="K4">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>59</v>
+      <c r="J4" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
       </c>
       <c r="M4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N4">
-        <v>6</v>
-      </c>
-      <c r="O4">
         <v>148.87</v>
       </c>
-      <c r="P4" s="2">
+      <c r="O4" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99520347622628891</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R4">
+      <c r="Q4">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>486</v>
       </c>
-      <c r="S4" s="2">
+      <c r="R4" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93217088055797737</v>
       </c>
-      <c r="T4" s="2" t="str">
+      <c r="S4" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="U4" s="3">
+      <c r="T4" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30631687242798356</v>
       </c>
-      <c r="V4" s="2">
+      <c r="U4" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1300634613198943</v>
       </c>
-      <c r="W4" t="s">
+      <c r="V4" t="s">
         <v>26</v>
       </c>
-      <c r="X4" s="2" t="str">
+      <c r="W4" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>grid</v>
+      </c>
+      <c r="X4" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Grid](#grid)</v>
       </c>
       <c r="Y4" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1367,97 +1379,98 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Grid
 Two-layer pattern of perpendicular lines, forming a grid. Overlapping points may cause noise or artifacts.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Print Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-grid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-grid.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5">
+      <c r="F5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
+      <c r="H5" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-Low</v>
+      </c>
       <c r="I5">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="J5">
         <v>2</v>
       </c>
-      <c r="K5">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>59</v>
+      <c r="J5" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5">
+        <v>8</v>
       </c>
       <c r="M5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N5">
-        <v>4</v>
-      </c>
-      <c r="O5">
         <v>148.54</v>
       </c>
-      <c r="P5" s="2">
+      <c r="O5" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R5">
+      <c r="Q5">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>484</v>
       </c>
-      <c r="S5" s="2">
+      <c r="R5" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92833478639930256</v>
       </c>
-      <c r="T5" s="2" t="str">
+      <c r="S5" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="U5" s="3">
+      <c r="T5" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30690082644628097</v>
       </c>
-      <c r="V5" s="2">
+      <c r="U5" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1322177830650146</v>
       </c>
-      <c r="W5" t="s">
+      <c r="V5" t="s">
         <v>26</v>
       </c>
-      <c r="X5" s="2" t="str">
+      <c r="W5" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-lattice</v>
+      </c>
+      <c r="X5" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[2D Lattice](#2d-lattice)</v>
       </c>
       <c r="Y5" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1466,97 +1479,98 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Lattice
 Low-strength pattern with good flexibility. Angle 1 and angle 2 TBD.
-- **Horizontal Strength (X-Y):** 0,925
-- **Vertical Strength (Z):** 0,75
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Normal-Low
+- **Vertical Strength (Z):** Low
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Print Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-2d-lattice](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-2d-lattice.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6">
+      <c r="F6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
+      <c r="H6" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I6">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J6">
         <v>2</v>
       </c>
-      <c r="K6">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>59</v>
+      <c r="J6" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
       </c>
       <c r="M6">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="N6">
-        <v>49</v>
-      </c>
-      <c r="O6">
         <v>154.68</v>
       </c>
-      <c r="P6" s="2">
+      <c r="O6" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0340436199548759</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>469</v>
       </c>
-      <c r="S6" s="2">
+      <c r="R6" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.8995640802092415</v>
       </c>
-      <c r="T6" s="2" t="str">
+      <c r="S6" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U6" s="3">
+      <c r="T6" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.3298081023454158</v>
       </c>
-      <c r="V6" s="2">
+      <c r="U6" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.2167272496405854</v>
       </c>
-      <c r="W6" t="s">
+      <c r="V6" t="s">
         <v>28</v>
       </c>
-      <c r="X6" s="2" t="str">
+      <c r="W6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>line</v>
+      </c>
+      <c r="X6" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Line](#line)</v>
       </c>
       <c r="Y6" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1565,97 +1579,98 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Line
 Similar to [rectilinear](#rectilinear), but each line is slightly rotated to improve print speed.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 0,75
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Low
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-line](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-line.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7">
+      <c r="F7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7">
         <v>6</v>
       </c>
+      <c r="H7" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I7">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J7">
         <v>6</v>
       </c>
-      <c r="K7">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>59</v>
+      <c r="J7" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
       </c>
       <c r="M7">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="N7">
-        <v>50</v>
-      </c>
-      <c r="O7">
         <v>148.54</v>
       </c>
-      <c r="P7" s="2">
+      <c r="O7" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R7">
+      <c r="Q7">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="S7" s="2">
+      <c r="R7" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="T7" s="2" t="str">
+      <c r="S7" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U7" s="3">
+      <c r="T7" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31604255319148933</v>
       </c>
-      <c r="V7" s="2">
+      <c r="U7" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1659434191563129</v>
       </c>
-      <c r="W7" t="s">
+      <c r="V7" t="s">
         <v>28</v>
       </c>
-      <c r="X7" s="2" t="str">
+      <c r="W7" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cubic</v>
+      </c>
+      <c r="X7" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Cubic](#cubic)</v>
       </c>
       <c r="Y7" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1664,25 +1679,25 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Cubic
 3D cube pattern with corners facing down, distributing force in all directions. Triangles in the horizontal plane provide good X-Y strength.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-cubic.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -1690,71 +1705,72 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8">
+      <c r="F8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8">
         <v>6</v>
       </c>
+      <c r="H8" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I8">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J8">
         <v>4</v>
       </c>
-      <c r="K8">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>59</v>
+      <c r="J8" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="N8">
-        <v>50</v>
-      </c>
-      <c r="O8">
         <v>147.55000000000001</v>
       </c>
-      <c r="P8" s="2">
+      <c r="O8" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9863792094927718</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R8">
+      <c r="Q8">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="S8" s="2">
+      <c r="R8" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="T8" s="2" t="str">
+      <c r="S8" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U8" s="3">
+      <c r="T8" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31393617021276599</v>
       </c>
-      <c r="V8" s="2">
+      <c r="U8" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.158172556190346</v>
       </c>
-      <c r="W8" t="s">
+      <c r="V8" t="s">
         <v>28</v>
       </c>
-      <c r="X8" s="2" t="str">
+      <c r="W8" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>triangles</v>
+      </c>
+      <c r="X8" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Triangles](#triangles)</v>
       </c>
       <c r="Y8" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1763,25 +1779,25 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Triangles
 Triangle-based grid, offering strong X-Y strength but with triple overlaps at intersections.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-triangles](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-triangles.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1789,71 +1805,72 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9">
+      <c r="F9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9">
         <v>6</v>
       </c>
+      <c r="H9" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I9">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>59</v>
+      <c r="J9" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="N9">
-        <v>43</v>
-      </c>
-      <c r="O9">
         <v>148.53</v>
       </c>
-      <c r="P9" s="2">
+      <c r="O9" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99293055903735272</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>463</v>
       </c>
-      <c r="S9" s="2">
+      <c r="R9" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.88805579773321708</v>
       </c>
-      <c r="T9" s="2" t="str">
+      <c r="S9" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U9" s="3">
+      <c r="T9" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32079913606911448</v>
       </c>
-      <c r="V9" s="2">
+      <c r="U9" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1834913931485316</v>
       </c>
-      <c r="W9" t="s">
+      <c r="V9" t="s">
         <v>28</v>
       </c>
-      <c r="X9" s="2" t="str">
+      <c r="W9" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tri-hexagon</v>
+      </c>
+      <c r="X9" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Tri-hexagon](#tri-hexagon)</v>
       </c>
       <c r="Y9" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1862,91 +1879,92 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Tri-hexagon
 Similar to the [triangles](#triangles) pattern but offset to prevent triple overlaps at intersections. This design combines triangles and hexagons, providing excellent X-Y strength.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,25
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** Normal-High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-tri-hexagon](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-tri-hexagon.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10">
+      <c r="F10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10">
         <v>6</v>
       </c>
+      <c r="H10" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I10">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J10">
         <v>6</v>
       </c>
-      <c r="K10">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>59</v>
+      <c r="J10" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
       </c>
       <c r="M10">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="N10">
-        <v>49</v>
-      </c>
-      <c r="O10">
         <v>141.77000000000001</v>
       </c>
-      <c r="P10" s="2">
+      <c r="O10" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.94773961728085576</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>649</v>
       </c>
-      <c r="S10" s="2">
+      <c r="R10" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2448125544899737</v>
       </c>
-      <c r="T10" s="2" t="str">
+      <c r="S10" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="U10" s="3">
+      <c r="T10" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21844375963020032</v>
       </c>
-      <c r="V10" s="2">
+      <c r="U10" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.8058821871442029</v>
       </c>
-      <c r="W10" t="s">
+      <c r="V10" t="s">
         <v>24</v>
       </c>
-      <c r="X10" s="2" t="str">
+      <c r="W10" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>gyroid</v>
+      </c>
+      <c r="X10" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Gyroid](#gyroid)</v>
       </c>
       <c r="Y10" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -1955,100 +1973,101 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Gyroid
 Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-High
+- **Print Time:** Normal-High
 - **Material/Time (Higher better):** Low
 ![infill-top-gyroid](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-gyroid.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11">
+      <c r="F11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11">
         <v>6</v>
       </c>
+      <c r="H11" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I11">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J11">
         <v>6</v>
       </c>
-      <c r="K11">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>59</v>
+      <c r="J11" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11">
+        <v>11</v>
       </c>
       <c r="M11">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="N11">
-        <v>29</v>
-      </c>
-      <c r="O11">
         <v>151.01</v>
       </c>
-      <c r="P11" s="2">
+      <c r="O11" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0095094844154757</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R11">
+      <c r="Q11">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>689</v>
       </c>
-      <c r="S11" s="2">
+      <c r="R11" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.3215344376634699</v>
       </c>
-      <c r="T11" s="2" t="str">
+      <c r="S11" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="U11" s="3">
+      <c r="T11" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21917271407837444</v>
       </c>
-      <c r="V11" s="2">
+      <c r="U11" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.80857144412283</v>
       </c>
-      <c r="W11" t="s">
+      <c r="V11" t="s">
         <v>24</v>
       </c>
-      <c r="X11" s="2" t="str">
+      <c r="W11" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tpms-d</v>
+      </c>
+      <c r="X11" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[TPMS-D](#tpms-d)</v>
       </c>
       <c r="Y11" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2057,23 +2076,23 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### TPMS-D
 Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** High
+- **Print Time:** High
 - **Material/Time (Higher better):** Low
 ![infill-top-tpms-d](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-tpms-d.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2081,76 +2100,77 @@
         <v>0.15</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12">
+      <c r="F12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12">
         <v>6</v>
       </c>
+      <c r="H12" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I12">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J12">
         <v>6</v>
       </c>
-      <c r="K12">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>59</v>
+      <c r="J12" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12">
+        <v>17</v>
       </c>
       <c r="M12">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="N12">
-        <v>36</v>
-      </c>
-      <c r="O12">
         <v>190.54</v>
       </c>
-      <c r="P12" s="2">
+      <c r="O12" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.2737695328820924</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R12">
+      <c r="Q12">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>1056</v>
       </c>
-      <c r="S12" s="2">
+      <c r="R12" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>2.0254577157802962</v>
       </c>
-      <c r="T12" s="2" t="str">
+      <c r="S12" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Ultra-High</v>
       </c>
-      <c r="U12" s="3">
+      <c r="T12" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18043560606060605</v>
       </c>
-      <c r="V12" s="2">
+      <c r="U12" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.6656625993664127</v>
       </c>
-      <c r="W12" t="s">
+      <c r="V12" t="s">
         <v>25</v>
       </c>
-      <c r="X12" s="2" t="str">
+      <c r="W12" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>honeycomb</v>
+      </c>
+      <c r="X12" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Honeycomb](#honeycomb)</v>
       </c>
       <c r="Y12" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2159,23 +2179,23 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Honeycomb
 Hexagonal pattern balancing strength and material use. Double walls in each hexagon increase material consumption.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** High
-- **Time:** Ultra-High
+- **Print Time:** Ultra-High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-honeycomb.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2183,76 +2203,77 @@
         <v>0.4</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13">
+      <c r="F13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13">
         <v>5</v>
       </c>
+      <c r="H13" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
       <c r="I13">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="J13">
         <v>5</v>
       </c>
-      <c r="K13">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>60</v>
+      <c r="J13" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="N13">
-        <v>29</v>
-      </c>
-      <c r="O13">
         <v>97.57</v>
       </c>
-      <c r="P13" s="2">
+      <c r="O13" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.65226038271914422</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R13">
+      <c r="Q13">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>329</v>
       </c>
-      <c r="S13" s="2">
+      <c r="R13" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.63103748910200519</v>
       </c>
-      <c r="T13" s="2" t="str">
+      <c r="S13" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Low</v>
       </c>
-      <c r="U13" s="3">
+      <c r="T13" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29656534954407293</v>
       </c>
-      <c r="V13" s="2">
+      <c r="U13" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0940881667956823</v>
       </c>
-      <c r="W13" t="s">
+      <c r="V13" t="s">
         <v>26</v>
       </c>
-      <c r="X13" s="2" t="str">
+      <c r="W13" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>adaptive-cubic</v>
+      </c>
+      <c r="X13" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Adaptive Cubic](#adaptive-cubic)</v>
       </c>
       <c r="Y13" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2261,17 +2282,17 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Adaptive Cubic
 [Cubic](#cubic) pattern with adaptive density: denser near walls, sparser in the center. Saves material and time while maintaining strength, ideal for large prints.
-- **Horizontal Strength (X-Y):** 1,25
-- **Vertical Strength (Z):** 1,25
-- **Density Calculation:** Cubic reduced in the center
+- **Horizontal Strength (X-Y):** Normal-High
+- **Vertical Strength (Z):** Normal-High
+- **Density Calculation:** Same as [Cubic](#cubic) but reduced in the center
 - **Material Usage:** Low
-- **Time:** Low
+- **Print Time:** Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-adaptive-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-adaptive-cubic.png?raw=true)
 </v>
@@ -2291,70 +2312,71 @@
         <v>13</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14">
+        <v>69</v>
+      </c>
+      <c r="G14">
         <v>3</v>
       </c>
+      <c r="H14" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-Low</v>
+      </c>
       <c r="I14">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="J14">
         <v>4</v>
       </c>
-      <c r="K14">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>59</v>
+      <c r="J14" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14">
+        <v>8</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
       <c r="N14">
-        <v>8</v>
-      </c>
-      <c r="O14">
         <v>148.6</v>
       </c>
-      <c r="P14" s="2">
+      <c r="O14" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R14">
+      <c r="Q14">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>488</v>
       </c>
-      <c r="S14" s="2">
+      <c r="R14" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93600697471665206</v>
       </c>
-      <c r="T14" s="2" t="str">
+      <c r="S14" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="U14" s="3">
+      <c r="T14" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30450819672131146</v>
       </c>
-      <c r="V14" s="2">
+      <c r="U14" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1233908992984614</v>
       </c>
-      <c r="W14" t="s">
+      <c r="V14" t="s">
         <v>26</v>
       </c>
-      <c r="X14" s="2" t="str">
+      <c r="W14" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>aligned-rectilinear</v>
+      </c>
+      <c r="X14" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Aligned Rectilinear](#aligned-rectilinear)</v>
       </c>
       <c r="Y14" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2363,24 +2385,24 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Aligned Rectilinear
 Parallel lines spaced by the infill spacing, each layer printed in the same direction as the previous layer. Good horizontal strength perpendicular to the lines, but terrible in parallel direction.
 Recommended with layer anchoring to improve not perpendicular strength.
-- **Horizontal Strength (X-Y):** 0,925
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Normal-Low
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal
+- **Print Time:** Normal
 - **Material/Time (Higher better):** Normal
 ![infill-top-aligned-rectilinear](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-aligned-rectilinear.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="165" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2391,73 +2413,74 @@
         <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15">
+        <v>78</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15">
         <v>3</v>
       </c>
+      <c r="H15" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-Low</v>
+      </c>
       <c r="I15">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="J15">
         <v>3</v>
       </c>
-      <c r="K15">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>59</v>
+      <c r="J15" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-Low</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15">
+        <v>8</v>
       </c>
       <c r="M15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="O15">
         <v>147.52000000000001</v>
       </c>
-      <c r="P15" s="2">
+      <c r="O15" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.98617865797610094</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R15">
+      <c r="Q15">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>482</v>
       </c>
-      <c r="S15" s="2">
+      <c r="R15" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92449869224062775</v>
       </c>
-      <c r="T15" s="2" t="str">
+      <c r="S15" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U15" s="3">
+      <c r="T15" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30605809128630707</v>
       </c>
-      <c r="V15" s="2">
+      <c r="U15" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1291087665609367</v>
       </c>
-      <c r="W15" t="s">
+      <c r="V15" t="s">
         <v>26</v>
       </c>
-      <c r="X15" s="2" t="str">
+      <c r="W15" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-honeycomb</v>
+      </c>
+      <c r="X15" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[2D Honeycomb](#2d-honeycomb)</v>
       </c>
       <c r="Y15" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2466,23 +2489,23 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Honeycomb
 Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve interlayer point of contact and reduce the risk of delamination.
-- **Horizontal Strength (X-Y):** 0,925
-- **Vertical Strength (Z):** 0,925
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Normal-Low
+- **Vertical Strength (Z):** Normal-Low
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-2d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-2d-honeycomb.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2495,71 +2518,72 @@
       <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16">
+      <c r="F16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16">
         <v>4</v>
       </c>
+      <c r="H16" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
       <c r="I16">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="J16">
         <v>5</v>
       </c>
-      <c r="K16">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>61</v>
+      <c r="J16" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16">
+        <v>12</v>
       </c>
       <c r="M16">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="N16">
-        <v>28</v>
-      </c>
-      <c r="O16">
         <v>123.92</v>
       </c>
-      <c r="P16" s="2">
+      <c r="O16" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.82841146486170303</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R16">
+      <c r="Q16">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>748</v>
       </c>
-      <c r="S16" s="2">
+      <c r="R16" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.4346992153443765</v>
       </c>
-      <c r="T16" s="2" t="str">
+      <c r="S16" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="U16" s="3">
+      <c r="T16" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16566844919786097</v>
       </c>
-      <c r="V16" s="2">
+      <c r="U16" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.61118364015697213</v>
       </c>
-      <c r="W16" t="s">
+      <c r="V16" t="s">
         <v>25</v>
       </c>
-      <c r="X16" s="2" t="str">
+      <c r="W16" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>3d-honeycomb</v>
+      </c>
+      <c r="X16" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[3D Honeycomb](#3d-honeycomb)</v>
       </c>
       <c r="Y16" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2568,17 +2592,17 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 3D Honeycomb
 This infill tries to generate a printable honeycomb structure by printing squares and octagons mantaining a vertical angle high enough to mantian contact with the previous layer.
-- **Horizontal Strength (X-Y):** 1,075
-- **Vertical Strength (Z):** 1,25
+- **Horizontal Strength (X-Y):** Normal
+- **Vertical Strength (Z):** Normal-High
 - **Density Calculation:** Unknown
 - **Material Usage:** Normal-Low
-- **Time:** High
+- **Print Time:** High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-3d-honeycomb](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-3d-honeycomb.png?raw=true)
 </v>
@@ -2598,70 +2622,71 @@
         <v>15</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17">
+        <v>86</v>
+      </c>
+      <c r="G17">
         <v>2</v>
       </c>
+      <c r="H17" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I17">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J17">
         <v>4</v>
       </c>
-      <c r="K17">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>59</v>
+      <c r="J17" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17">
+        <v>13</v>
       </c>
       <c r="M17">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="N17">
-        <v>24</v>
-      </c>
-      <c r="O17">
         <v>148.63</v>
       </c>
-      <c r="P17" s="2">
+      <c r="O17" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99359906409292209</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R17">
+      <c r="Q17">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>804</v>
       </c>
-      <c r="S17" s="2">
+      <c r="R17" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.5421098517872711</v>
       </c>
-      <c r="T17" s="2" t="str">
+      <c r="S17" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="U17" s="3">
+      <c r="T17" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18486318407960198</v>
       </c>
-      <c r="V17" s="2">
+      <c r="U17" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.68199680943375651</v>
       </c>
-      <c r="W17" t="s">
+      <c r="V17" t="s">
         <v>25</v>
       </c>
-      <c r="X17" s="2" t="str">
+      <c r="W17" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>hilbert-curve</v>
+      </c>
+      <c r="X17" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Hilbert Curve](#hilbert-curve)</v>
       </c>
       <c r="Y17" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2670,24 +2695,24 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Hilbert Curve
 Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its Esthetic appeal and ability to fill space efficiently.
 Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for Esthetic purposes.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** High
+- **Print Time:** High
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-hilbert-curve](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-hilbert-curve.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="105" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2700,71 +2725,72 @@
       <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18">
+      <c r="F18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18">
         <v>2</v>
       </c>
+      <c r="H18" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I18">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J18">
         <v>4</v>
       </c>
-      <c r="K18">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>59</v>
+      <c r="J18" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18">
+        <v>7</v>
       </c>
       <c r="M18">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="N18">
-        <v>46</v>
-      </c>
-      <c r="O18">
         <v>148.21</v>
       </c>
-      <c r="P18" s="2">
+      <c r="O18" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99079134285953041</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R18">
+      <c r="Q18">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>466</v>
       </c>
-      <c r="S18" s="2">
+      <c r="R18" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.89380993897122929</v>
       </c>
-      <c r="T18" s="2" t="str">
+      <c r="S18" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U18" s="3">
+      <c r="T18" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31804721030042921</v>
       </c>
-      <c r="V18" s="2">
+      <c r="U18" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1733389952906987</v>
       </c>
-      <c r="W18" t="s">
+      <c r="V18" t="s">
         <v>28</v>
       </c>
-      <c r="X18" s="2" t="str">
+      <c r="W18" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>archimedean-chords</v>
+      </c>
+      <c r="X18" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Archimedean Chords](#archimedean-chords)</v>
       </c>
       <c r="Y18" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2773,23 +2799,23 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Archimedean Chords
 Spiral pattern that fills the area with concentric arcs, creating a smooth and continuous infill. Can be filled with resin thanks to its interconnected hollow structure, which allows the resin to flow through it and cure properly.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal-High
 ![infill-top-archimedean-chords](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-archimedean-chords.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2797,76 +2823,77 @@
         <v>1.85</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19">
+      <c r="F19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19">
         <v>2</v>
       </c>
+      <c r="H19" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I19">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J19">
         <v>4</v>
       </c>
-      <c r="K19">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.075</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>59</v>
+      <c r="J19" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19">
+        <v>9</v>
       </c>
       <c r="M19">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="N19">
-        <v>30</v>
-      </c>
-      <c r="O19">
         <v>148.72</v>
       </c>
-      <c r="P19" s="2">
+      <c r="O19" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99420071864293469</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R19">
+      <c r="Q19">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>570</v>
       </c>
-      <c r="S19" s="2">
+      <c r="R19" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.0932868352223191</v>
       </c>
-      <c r="T19" s="2" t="str">
+      <c r="S19" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="U19" s="3">
+      <c r="T19" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.26091228070175437</v>
       </c>
-      <c r="V19" s="2">
+      <c r="U19" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.96255695187019885</v>
       </c>
-      <c r="W19" t="s">
+      <c r="V19" t="s">
         <v>26</v>
       </c>
-      <c r="X19" s="2" t="str">
+      <c r="W19" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>octagram-spiral</v>
+      </c>
+      <c r="X19" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Octagram Spiral](#octagram-spiral)</v>
       </c>
       <c r="Y19" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2875,23 +2902,23 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Octagram Spiral
 Esthetic pattern with low strength and high print time.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 1,075
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Normal
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-High
+- **Print Time:** Normal-High
 - **Material/Time (Higher better):** Normal
 ![infill-top-octagram-spiral](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-octagram-spiral.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="120" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2899,76 +2926,77 @@
         <v>9.99</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20">
+      <c r="F20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20">
         <v>2</v>
       </c>
+      <c r="H20" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I20">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J20">
         <v>2</v>
       </c>
-      <c r="K20">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>31</v>
+      <c r="J20" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="N20">
-        <v>50</v>
-      </c>
-      <c r="O20">
         <v>49.39</v>
       </c>
-      <c r="P20" s="2">
+      <c r="O20" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.33017464694576754</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="R20">
+      <c r="P20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q20">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>170</v>
       </c>
-      <c r="S20" s="2">
+      <c r="R20" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.32606800348735832</v>
       </c>
-      <c r="T20" s="2" t="str">
+      <c r="S20" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Extra-Low</v>
       </c>
-      <c r="U20" s="3">
+      <c r="T20" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29052941176470587</v>
       </c>
-      <c r="V20" s="2">
+      <c r="U20" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0718203998091715</v>
       </c>
-      <c r="W20" t="s">
+      <c r="V20" t="s">
         <v>26</v>
       </c>
-      <c r="X20" s="2" t="str">
+      <c r="W20" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>support-cubic</v>
+      </c>
+      <c r="X20" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Support Cubic](#support-cubic)</v>
       </c>
       <c r="Y20" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -2977,91 +3005,92 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Support Cubic
 Support |Cubic is a variation of the [Cubic](#cubic) infill pattern that is specifically designed for support top layers. Will use more material than Lightning infill but will provide better strength. Nevertheless, it is still a low-density infill pattern.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 0,75
-- **Density Calculation:** before top shell layers
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Low
+- **Density Calculation:** % of layer before top shell layers
 - **Material Usage:** Extra-Low
-- **Time:** Extra-Low
+- **Print Time:** Extra-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-support-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-support-cubic.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="F21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21">
+      <c r="F21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21">
         <v>2</v>
       </c>
+      <c r="H21" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
       <c r="I21">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="J21">
         <v>2</v>
       </c>
-      <c r="K21">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>0.75</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>31</v>
+      <c r="J21" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Low</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="N21">
-        <v>16</v>
-      </c>
-      <c r="O21">
         <v>12.33</v>
       </c>
-      <c r="P21" s="2">
+      <c r="O21" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>8.2426673351717217E-2</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R21">
+      <c r="P21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q21">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>76</v>
       </c>
-      <c r="S21" s="2">
+      <c r="R21" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.14577157802964255</v>
       </c>
-      <c r="T21" s="2" t="str">
+      <c r="S21" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Ultra-Low</v>
       </c>
-      <c r="U21" s="3">
+      <c r="T21" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16223684210526315</v>
       </c>
-      <c r="V21" s="2">
+      <c r="U21" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.59852376361078963</v>
       </c>
-      <c r="W21" t="s">
+      <c r="V21" t="s">
         <v>25</v>
       </c>
-      <c r="X21" s="2" t="str">
+      <c r="W21" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>lightning</v>
+      </c>
+      <c r="X21" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Lightning](#lightning)</v>
       </c>
       <c r="Y21" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -3070,91 +3099,92 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Lightning
 Ultra-fast, ultra-low material infill. Designed for speed and efficiency, ideal for quick prints or non-structural prototypes.
-- **Horizontal Strength (X-Y):** 0,75
-- **Vertical Strength (Z):** 0,75
-- **Density Calculation:** before top shell layers
+- **Horizontal Strength (X-Y):** Low
+- **Vertical Strength (Z):** Low
+- **Density Calculation:** % of layer before top shell layers
 - **Material Usage:** Ultra-Low
-- **Time:** Ultra-Low
+- **Print Time:** Ultra-Low
 - **Material/Time (Higher better):** Extra Low
 ![infill-top-lightning](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-lightning.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22">
+      <c r="F22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22">
         <v>5</v>
       </c>
+      <c r="H22" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
       <c r="I22">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="J22">
         <v>5</v>
       </c>
-      <c r="K22">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.25</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>59</v>
+      <c r="J22" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>Normal-High</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
       </c>
       <c r="M22">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="N22">
-        <v>40</v>
-      </c>
-      <c r="O22">
         <v>144.69999999999999</v>
       </c>
-      <c r="P22" s="2">
+      <c r="O22" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.96732681540904142</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="P22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R22">
+      <c r="Q22">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>640</v>
       </c>
-      <c r="S22" s="2">
+      <c r="R22" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2275501307759371</v>
       </c>
-      <c r="T22" s="2" t="str">
+      <c r="S22" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="U22" s="3">
+      <c r="T22" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.22609374999999998</v>
       </c>
-      <c r="V22" s="2">
+      <c r="U22" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.83410451302470801</v>
       </c>
-      <c r="W22" t="s">
+      <c r="V22" t="s">
         <v>24</v>
       </c>
-      <c r="X22" s="2" t="str">
+      <c r="W22" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cross-hatch</v>
+      </c>
+      <c r="X22" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Cross Hatch](#cross-hatch)</v>
       </c>
       <c r="Y22" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -3163,91 +3193,92 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Cross Hatch
 Similar to [Gyroid](#gyroid) but with linear patterns, creating weak points at internal corners.
-- **Horizontal Strength (X-Y):** 1,25
-- **Vertical Strength (Z):** 1,25
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** Normal-High
+- **Vertical Strength (Z):** Normal-High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-High
+- **Print Time:** Normal-High
 - **Material/Time (Higher better):** Low
 ![infill-top-cross-hatch](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-cross-hatch.png?raw=true)
 </v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23">
+        <v>45</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23">
         <v>6</v>
       </c>
+      <c r="H23" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
       <c r="I23">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="J23">
         <v>6</v>
       </c>
-      <c r="K23">
-        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Max %])</f>
-        <v>1.6</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>59</v>
+      <c r="J23" t="str">
+        <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
+        <v>High</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23">
+        <v>8</v>
       </c>
       <c r="M23">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
         <v>148.55000000000001</v>
       </c>
-      <c r="P23" s="2">
+      <c r="O23" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99306426004846671</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R23">
+      <c r="Q23">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>481</v>
       </c>
-      <c r="S23" s="2">
+      <c r="R23" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92258064516129035</v>
       </c>
-      <c r="T23" s="2" t="str">
+      <c r="S23" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="U23" s="3">
+      <c r="T23" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30883575883575887</v>
       </c>
-      <c r="V23" s="2">
+      <c r="U23" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1393561309338132</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X23" s="2" t="str">
+      <c r="W23" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>quarter-cubic</v>
+      </c>
+      <c r="X23" s="2" t="str">
+        <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
+        <v>[Quarter Cubic](#quarter-cubic)</v>
       </c>
       <c r="Y23" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -3256,17 +3287,17 @@
 - **Vertical Strength (Z):** "&amp;Infill[[#This Row],[Z Strength]]&amp;"
 - **Density Calculation:** "&amp;Infill[[#This Row],[DensityCalc]]&amp;"
 - **Material Usage:** "&amp;Infill[[#This Row],[Material Usage]]&amp;"
-- **Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
+- **Print Time:** "&amp;Infill[[#This Row],[Time]]&amp;"
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Quarter Cubic
 [Cubic](#cubic) pattern with extra internal divisions, improving X-Y strength.
-- **Horizontal Strength (X-Y):** 1,6
-- **Vertical Strength (Z):** 1,6
-- **Density Calculation:** Total infill material usage
+- **Horizontal Strength (X-Y):** High
+- **Vertical Strength (Z):** High
+- **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
-- **Time:** Normal-Low
+- **Print Time:** Normal-Low
 - **Material/Time (Higher better):** Normal
 ![infill-top-quarter-cubic](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-quarter-cubic.png?raw=true)
 </v>
@@ -3274,7 +3305,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="P2:P23">
+  <conditionalFormatting sqref="O2:O23">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3286,7 +3317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S23">
+  <conditionalFormatting sqref="R2:R23">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3298,7 +3329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U23">
+  <conditionalFormatting sqref="T2:T23">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3310,7 +3341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V23">
+  <conditionalFormatting sqref="U2:U23">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Update 3D Honeycomb infill strength ratings
Adjusted the horizontal strength rating for 3D Honeycomb infill from 'Normal' to 'Normal-High' in the strength settings documentation and table. Updated the infill_desc_calculator.xlsx file to reflect these changes.
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207EB570-29FA-4B00-968A-CB3FC33489BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6190A67-761B-4BA2-BCD4-C6D7D3DAB68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
@@ -399,6 +399,9 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -419,28 +422,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -588,6 +569,25 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -606,46 +606,46 @@
   <autoFilter ref="E1:Y23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{3D89DC5A-8AB2-4952-BD08-8DD7EDC3072E}" name="Infill" totalsRowLabel="Total"/>
-    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="2" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{94F205F5-D170-40A1-8C5F-879C636804AA}" name="X-Y Strength" dataDxfId="20">
+    <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="21" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{94F205F5-D170-40A1-8C5F-879C636804AA}" name="X-Y Strength" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{D6A80A00-4E52-418C-9F58-C091734E73D4}" name="Z Strength" dataDxfId="18">
+    <tableColumn id="20" xr3:uid="{E9317962-9E1D-4D5B-9028-66E03DB4FC89}" name="Z-N" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{D6A80A00-4E52-418C-9F58-C091734E73D4}" name="Z Strength" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="17" dataCellStyle="Porcentaje"/>
+    <tableColumn id="15" xr3:uid="{A5F7A5DA-C5EE-4BAA-9BF1-1AF83AB88E06}" name="DensityCalc" dataDxfId="16" dataCellStyle="Porcentaje"/>
     <tableColumn id="5" xr3:uid="{CC2FB322-5D42-4375-BC4F-16927902366E}" name="hs"/>
     <tableColumn id="2" xr3:uid="{0B06FA91-5EDF-466A-8753-FFCA36B0EFB0}" name="min"/>
-    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Effective" totalsRowFunction="average" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Porcentaje">
+    <tableColumn id="3" xr3:uid="{E842218B-6949-43A1-A35A-6C35A7D812BB}" name="g" totalsRowFunction="average" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{55891199-0C82-4B3C-B416-4BE5775CD688}" name="% Effective" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/(997.25*0.15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{32CE485A-842B-45B3-8F5D-B93DF0C49C8F}" name="Material Usage" dataDxfId="13" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="11" xr3:uid="{32CE485A-842B-45B3-8F5D-B93DF0C49C8F}" name="Material Usage" dataDxfId="12" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{C7DC0832-87AA-48F2-8845-AAE7F7254500}" name="Total Time" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="t prom" dataDxfId="10" dataCellStyle="Porcentaje">
+    <tableColumn id="8" xr3:uid="{252F6390-A339-497F-955E-B7D85B035B56}" name="t prom" dataDxfId="9" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="9" dataCellStyle="Porcentaje">
+    <tableColumn id="12" xr3:uid="{0224A6DD-647D-41E2-B74E-256AAEBCEDB8}" name="Time" dataDxfId="8" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Porcentaje">
+    <tableColumn id="7" xr3:uid="{3A33F243-4754-4015-A3B1-EEAA7B810730}" name="g/t" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/t prom" dataDxfId="6" dataCellStyle="Porcentaje">
+    <tableColumn id="10" xr3:uid="{81F5FB07-EC80-4D98-B9AE-8EF8E1629F1A}" name="g/t prom" dataDxfId="5" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="5" dataCellStyle="Porcentaje"/>
-    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="4" dataCellStyle="Porcentaje">
+    <tableColumn id="13" xr3:uid="{F80BCD33-B1E3-433F-AF6D-F982D670E727}" name="Material/Time" dataDxfId="4" dataCellStyle="Porcentaje"/>
+    <tableColumn id="19" xr3:uid="{44AE3D7E-C8D1-4165-B6BD-E525E4F90672}" name="image" dataDxfId="3" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{75AA760A-15C0-4692-B168-BF74BE6D50F6}" name="Ref" dataDxfId="1" dataCellStyle="Porcentaje">
+    <tableColumn id="21" xr3:uid="{75AA760A-15C0-4692-B168-BF74BE6D50F6}" name="Ref" dataDxfId="2" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="MD" dataDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="MD" dataDxfId="1" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -678,7 +678,7 @@
   <autoFilter ref="A11:C20" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1D00CA6A-CEDD-45A1-8BA8-6DB7769D516C}" name="N"/>
-    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="3" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="0" dataCellStyle="Porcentaje"/>
     <tableColumn id="3" xr3:uid="{18E14714-6899-4575-90B8-4F97863AF141}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,11 +2522,11 @@
         <v>70</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
-        <v>Normal</v>
+        <v>Normal-High</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -2598,7 +2598,7 @@
 "</f>
         <v xml:space="preserve">### 3D Honeycomb
 This infill tries to generate a printable honeycomb structure by printing squares and octagons mantaining a vertical angle high enough to mantian contact with the previous layer.
-- **Horizontal Strength (X-Y):** Normal
+- **Horizontal Strength (X-Y):** Normal-High
 - **Vertical Strength (Z):** Normal-High
 - **Density Calculation:** Unknown
 - **Material Usage:** Normal-Low

</xml_diff>

<commit_message>
Added Old and New Order in xlsx
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6190A67-761B-4BA2-BCD4-C6D7D3DAB68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D2D728-191F-46BB-9A0E-F14B1B1CC376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
   <si>
     <t>Infill</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>MD</t>
+  </si>
+  <si>
+    <t>Current Order</t>
+  </si>
+  <si>
+    <t>Tentative Order</t>
   </si>
 </sst>
 </file>
@@ -602,9 +608,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}" name="Infill" displayName="Infill" ref="E1:Y23">
-  <autoFilter ref="E1:Y23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}" name="Infill" displayName="Infill" ref="E1:AA23">
+  <autoFilter ref="E1:AA23" xr:uid="{14E0E815-2798-4AE1-A846-B8CADCC14BD7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:AA23">
+    <sortCondition ref="E1:E23"/>
+  </sortState>
+  <tableColumns count="23">
+    <tableColumn id="22" xr3:uid="{8D3A2FCE-7458-4DCB-BCE6-4671B3808244}" name="Current Order"/>
+    <tableColumn id="23" xr3:uid="{061A8DA1-BAF1-41F8-8DD1-5E8F3141DA90}" name="Tentative Order"/>
     <tableColumn id="1" xr3:uid="{3D89DC5A-8AB2-4952-BD08-8DD7EDC3072E}" name="Infill" totalsRowLabel="Total"/>
     <tableColumn id="18" xr3:uid="{0AF02225-407A-4366-B524-2DC6A8FF6278}" name="Desc" dataDxfId="21" dataCellStyle="Porcentaje"/>
     <tableColumn id="9" xr3:uid="{EDA17F6B-F438-45F7-B1D4-D47E28684329}" name="XY-N" dataDxfId="20"/>
@@ -1002,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,16 +1024,17 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="23" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.85546875" customWidth="1"/>
-    <col min="25" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" customWidth="1"/>
+    <col min="26" max="28" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1030,148 +1042,160 @@
         <v>42</v>
       </c>
       <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>90</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>89</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>77</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>2</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>4</v>
       </c>
-      <c r="J2" t="str">
+      <c r="L2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>8</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>13</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>158.77000000000001</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0613854767276678</v>
       </c>
-      <c r="P2" s="2" t="str">
+      <c r="R2" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[% Effective]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>493</v>
       </c>
-      <c r="R2" s="2">
+      <c r="T2" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.94559721011333908</v>
       </c>
-      <c r="S2" s="2" t="str">
+      <c r="U2" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="T2" s="3">
+      <c r="V2" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32204868154158217</v>
       </c>
-      <c r="U2" s="2">
+      <c r="W2" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1881012132687909</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="2" t="str">
+      <c r="Y2" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>concentric</v>
       </c>
-      <c r="X2" s="2" t="str">
+      <c r="Z2" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Concentric](#concentric)</v>
       </c>
-      <c r="Y2" s="2" t="str">
+      <c r="AA2" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1194,85 +1218,91 @@
 </v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="H3" t="str">
+      <c r="J3" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-Low</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="J3" t="str">
+      <c r="L3" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>8</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>7</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>148.6</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>487</v>
       </c>
-      <c r="R3" s="2">
+      <c r="T3" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93408892763731477</v>
       </c>
-      <c r="S3" s="2" t="str">
+      <c r="U3" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="T3" s="3">
+      <c r="V3" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30513347022587267</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1256976567918875</v>
       </c>
-      <c r="V3" t="str">
+      <c r="X3" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[g/t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="W3" s="2" t="str">
+      <c r="Y3" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>rectilinear</v>
       </c>
-      <c r="X3" s="2" t="str">
+      <c r="Z3" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Rectilinear](#rectilinear)</v>
       </c>
-      <c r="Y3" s="2" t="str">
+      <c r="AA3" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1295,84 +1325,90 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="2">
         <v>0.15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>6</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>6</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>8</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>148.87</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99520347622628891</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>486</v>
       </c>
-      <c r="R4" s="2">
+      <c r="T4" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93217088055797737</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="U4" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="T4" s="3">
+      <c r="V4" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30631687242798356</v>
       </c>
-      <c r="U4" s="2">
+      <c r="W4" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1300634613198943</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="2" t="str">
+      <c r="Y4" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>grid</v>
       </c>
-      <c r="X4" s="2" t="str">
+      <c r="Z4" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Grid](#grid)</v>
       </c>
-      <c r="Y4" s="2" t="str">
+      <c r="AA4" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1395,84 +1431,90 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-Low</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>2</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>8</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>4</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>148.54</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>484</v>
       </c>
-      <c r="R5" s="2">
+      <c r="T5" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92833478639930256</v>
       </c>
-      <c r="S5" s="2" t="str">
+      <c r="U5" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="T5" s="3">
+      <c r="V5" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30690082644628097</v>
       </c>
-      <c r="U5" s="2">
+      <c r="W5" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1322177830650146</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="2" t="str">
+      <c r="Y5" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-lattice</v>
       </c>
-      <c r="X5" s="2" t="str">
+      <c r="Z5" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[2D Lattice](#2d-lattice)</v>
       </c>
-      <c r="Y5" s="2" t="str">
+      <c r="AA5" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1495,84 +1537,90 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>7</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>49</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>154.68</v>
       </c>
-      <c r="O6" s="2">
+      <c r="Q6" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0340436199548759</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>469</v>
       </c>
-      <c r="R6" s="2">
+      <c r="T6" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.8995640802092415</v>
       </c>
-      <c r="S6" s="2" t="str">
+      <c r="U6" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T6" s="3">
+      <c r="V6" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.3298081023454158</v>
       </c>
-      <c r="U6" s="2">
+      <c r="W6" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.2167272496405854</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>28</v>
       </c>
-      <c r="W6" s="2" t="str">
+      <c r="Y6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>line</v>
       </c>
-      <c r="X6" s="2" t="str">
+      <c r="Z6" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Line](#line)</v>
       </c>
-      <c r="Y6" s="2" t="str">
+      <c r="AA6" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1595,84 +1643,90 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>6</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>6</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>7</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>50</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>148.54</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9929974095429096</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="R7" s="2">
+      <c r="T7" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="S7" s="2" t="str">
+      <c r="U7" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T7" s="3">
+      <c r="V7" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31604255319148933</v>
       </c>
-      <c r="U7" s="2">
+      <c r="W7" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1659434191563129</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="2" t="str">
+      <c r="Y7" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cubic</v>
       </c>
-      <c r="X7" s="2" t="str">
+      <c r="Z7" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Cubic](#cubic)</v>
       </c>
-      <c r="Y7" s="2" t="str">
+      <c r="AA7" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1695,84 +1749,90 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
         <v>7</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>4</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>7</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>50</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>147.55000000000001</v>
       </c>
-      <c r="O8" s="2">
+      <c r="Q8" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.9863792094927718</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>470</v>
       </c>
-      <c r="R8" s="2">
+      <c r="T8" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.9014821272885789</v>
       </c>
-      <c r="S8" s="2" t="str">
+      <c r="U8" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T8" s="3">
+      <c r="V8" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31393617021276599</v>
       </c>
-      <c r="U8" s="2">
+      <c r="W8" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.158172556190346</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="2" t="str">
+      <c r="Y8" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>triangles</v>
       </c>
-      <c r="X8" s="2" t="str">
+      <c r="Z8" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Triangles](#triangles)</v>
       </c>
-      <c r="Y8" s="2" t="str">
+      <c r="AA8" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1795,84 +1855,90 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>6</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>7</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>43</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>148.53</v>
       </c>
-      <c r="O9" s="2">
+      <c r="Q9" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99293055903735272</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>463</v>
       </c>
-      <c r="R9" s="2">
+      <c r="T9" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.88805579773321708</v>
       </c>
-      <c r="S9" s="2" t="str">
+      <c r="U9" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T9" s="3">
+      <c r="V9" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.32079913606911448</v>
       </c>
-      <c r="U9" s="2">
+      <c r="W9" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1834913931485316</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>28</v>
       </c>
-      <c r="W9" s="2" t="str">
+      <c r="Y9" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tri-hexagon</v>
       </c>
-      <c r="X9" s="2" t="str">
+      <c r="Z9" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Tri-hexagon](#tri-hexagon)</v>
       </c>
-      <c r="Y9" s="2" t="str">
+      <c r="AA9" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1895,78 +1961,84 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+    <row r="10" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+      <c r="E10">
         <v>9</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>6</v>
       </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>6</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>10</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>49</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>141.77000000000001</v>
       </c>
-      <c r="O10" s="2">
+      <c r="Q10" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.94773961728085576</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>649</v>
       </c>
-      <c r="R10" s="2">
+      <c r="T10" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2448125544899737</v>
       </c>
-      <c r="S10" s="2" t="str">
+      <c r="U10" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="T10" s="3">
+      <c r="V10" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21844375963020032</v>
       </c>
-      <c r="U10" s="2">
+      <c r="W10" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.8058821871442029</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>24</v>
       </c>
-      <c r="W10" s="2" t="str">
+      <c r="Y10" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>gyroid</v>
       </c>
-      <c r="X10" s="2" t="str">
+      <c r="Z10" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Gyroid](#gyroid)</v>
       </c>
-      <c r="Y10" s="2" t="str">
+      <c r="AA10" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1989,7 +2061,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1999,77 +2071,83 @@
       <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
         <v>10</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>6</v>
       </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>6</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>11</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>29</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>151.01</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.0095094844154757</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>689</v>
       </c>
-      <c r="R11" s="2">
+      <c r="T11" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.3215344376634699</v>
       </c>
-      <c r="S11" s="2" t="str">
+      <c r="U11" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="T11" s="3">
+      <c r="V11" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.21917271407837444</v>
       </c>
-      <c r="U11" s="2">
+      <c r="W11" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.80857144412283</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>24</v>
       </c>
-      <c r="W11" s="2" t="str">
+      <c r="Y11" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>tpms-d</v>
       </c>
-      <c r="X11" s="2" t="str">
+      <c r="Z11" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[TPMS-D](#tpms-d)</v>
       </c>
-      <c r="Y11" s="2" t="str">
+      <c r="AA11" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2092,7 +2170,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2102,77 +2180,83 @@
       <c r="C12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
         <v>11</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>6</v>
       </c>
-      <c r="H12" t="str">
+      <c r="J12" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>6</v>
       </c>
-      <c r="J12" t="str">
+      <c r="L12" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>17</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>36</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>190.54</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>1.2737695328820924</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>1056</v>
       </c>
-      <c r="R12" s="2">
+      <c r="T12" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>2.0254577157802962</v>
       </c>
-      <c r="S12" s="2" t="str">
+      <c r="U12" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Ultra-High</v>
       </c>
-      <c r="T12" s="3">
+      <c r="V12" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18043560606060605</v>
       </c>
-      <c r="U12" s="2">
+      <c r="W12" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.6656625993664127</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>25</v>
       </c>
-      <c r="W12" s="2" t="str">
+      <c r="Y12" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>honeycomb</v>
       </c>
-      <c r="X12" s="2" t="str">
+      <c r="Z12" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Honeycomb](#honeycomb)</v>
       </c>
-      <c r="Y12" s="2" t="str">
+      <c r="AA12" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2195,7 +2279,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2205,77 +2289,83 @@
       <c r="C13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
         <v>12</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>5</v>
       </c>
-      <c r="H13" t="str">
+      <c r="J13" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>5</v>
       </c>
-      <c r="J13" t="str">
+      <c r="L13" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>5</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>29</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>97.57</v>
       </c>
-      <c r="O13" s="2">
+      <c r="Q13" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.65226038271914422</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>329</v>
       </c>
-      <c r="R13" s="2">
+      <c r="T13" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.63103748910200519</v>
       </c>
-      <c r="S13" s="2" t="str">
+      <c r="U13" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Low</v>
       </c>
-      <c r="T13" s="3">
+      <c r="V13" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29656534954407293</v>
       </c>
-      <c r="U13" s="2">
+      <c r="W13" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0940881667956823</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>26</v>
       </c>
-      <c r="W13" s="2" t="str">
+      <c r="Y13" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>adaptive-cubic</v>
       </c>
-      <c r="X13" s="2" t="str">
+      <c r="Z13" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Adaptive Cubic](#adaptive-cubic)</v>
       </c>
-      <c r="Y13" s="2" t="str">
+      <c r="AA13" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2298,7 +2388,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="255" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2308,77 +2398,83 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
         <v>13</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>3</v>
       </c>
-      <c r="H14" t="str">
+      <c r="J14" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-Low</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>4</v>
       </c>
-      <c r="J14" t="str">
+      <c r="L14" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>8</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>8</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>148.6</v>
       </c>
-      <c r="O14" s="2">
+      <c r="Q14" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99339851257625134</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>488</v>
       </c>
-      <c r="R14" s="2">
+      <c r="T14" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.93600697471665206</v>
       </c>
-      <c r="S14" s="2" t="str">
+      <c r="U14" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal</v>
       </c>
-      <c r="T14" s="3">
+      <c r="V14" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30450819672131146</v>
       </c>
-      <c r="U14" s="2">
+      <c r="W14" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1233908992984614</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="2" t="str">
+      <c r="Y14" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>aligned-rectilinear</v>
       </c>
-      <c r="X14" s="2" t="str">
+      <c r="Z14" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Aligned Rectilinear](#aligned-rectilinear)</v>
       </c>
-      <c r="Y14" s="2" t="str">
+      <c r="AA14" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2402,7 +2498,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="300" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2412,77 +2508,83 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="H15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>3</v>
       </c>
-      <c r="H15" t="str">
+      <c r="J15" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-Low</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>3</v>
       </c>
-      <c r="J15" t="str">
+      <c r="L15" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal-Low</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>8</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>2</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>147.52000000000001</v>
       </c>
-      <c r="O15" s="2">
+      <c r="Q15" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.98617865797610094</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>482</v>
       </c>
-      <c r="R15" s="2">
+      <c r="T15" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92449869224062775</v>
       </c>
-      <c r="S15" s="2" t="str">
+      <c r="U15" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T15" s="3">
+      <c r="V15" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30605809128630707</v>
       </c>
-      <c r="U15" s="2">
+      <c r="W15" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1291087665609367</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>26</v>
       </c>
-      <c r="W15" s="2" t="str">
+      <c r="Y15" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>2d-honeycomb</v>
       </c>
-      <c r="X15" s="2" t="str">
+      <c r="Z15" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[2D Honeycomb](#2d-honeycomb)</v>
       </c>
-      <c r="Y15" s="2" t="str">
+      <c r="AA15" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2505,7 +2607,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="180" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2515,77 +2617,83 @@
       <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>5</v>
       </c>
-      <c r="H16" t="str">
+      <c r="J16" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>5</v>
       </c>
-      <c r="J16" t="str">
+      <c r="L16" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>12</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>28</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>123.92</v>
       </c>
-      <c r="O16" s="2">
+      <c r="Q16" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.82841146486170303</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="R16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>748</v>
       </c>
-      <c r="R16" s="2">
+      <c r="T16" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.4346992153443765</v>
       </c>
-      <c r="S16" s="2" t="str">
+      <c r="U16" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="T16" s="3">
+      <c r="V16" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16566844919786097</v>
       </c>
-      <c r="U16" s="2">
+      <c r="W16" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.61118364015697213</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>25</v>
       </c>
-      <c r="W16" s="2" t="str">
+      <c r="Y16" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>3d-honeycomb</v>
       </c>
-      <c r="X16" s="2" t="str">
+      <c r="Z16" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[3D Honeycomb](#3d-honeycomb)</v>
       </c>
-      <c r="Y16" s="2" t="str">
+      <c r="AA16" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2608,7 +2716,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="300" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -2618,77 +2726,83 @@
       <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>2</v>
       </c>
-      <c r="H17" t="str">
+      <c r="J17" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>4</v>
       </c>
-      <c r="J17" t="str">
+      <c r="L17" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>13</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>24</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>148.63</v>
       </c>
-      <c r="O17" s="2">
+      <c r="Q17" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99359906409292209</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="R17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>804</v>
       </c>
-      <c r="R17" s="2">
+      <c r="T17" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.5421098517872711</v>
       </c>
-      <c r="S17" s="2" t="str">
+      <c r="U17" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>High</v>
       </c>
-      <c r="T17" s="3">
+      <c r="V17" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.18486318407960198</v>
       </c>
-      <c r="U17" s="2">
+      <c r="W17" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.68199680943375651</v>
       </c>
-      <c r="V17" t="s">
+      <c r="X17" t="s">
         <v>25</v>
       </c>
-      <c r="W17" s="2" t="str">
+      <c r="Y17" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>hilbert-curve</v>
       </c>
-      <c r="X17" s="2" t="str">
+      <c r="Z17" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Hilbert Curve](#hilbert-curve)</v>
       </c>
-      <c r="Y17" s="2" t="str">
+      <c r="AA17" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2712,7 +2826,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="195" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2722,77 +2836,83 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>2</v>
       </c>
-      <c r="H18" t="str">
+      <c r="J18" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>4</v>
       </c>
-      <c r="J18" t="str">
+      <c r="L18" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>7</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>46</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>148.21</v>
       </c>
-      <c r="O18" s="2">
+      <c r="Q18" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99079134285953041</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>466</v>
       </c>
-      <c r="R18" s="2">
+      <c r="T18" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.89380993897122929</v>
       </c>
-      <c r="S18" s="2" t="str">
+      <c r="U18" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T18" s="3">
+      <c r="V18" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.31804721030042921</v>
       </c>
-      <c r="U18" s="2">
+      <c r="W18" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1733389952906987</v>
       </c>
-      <c r="V18" t="s">
+      <c r="X18" t="s">
         <v>28</v>
       </c>
-      <c r="W18" s="2" t="str">
+      <c r="Y18" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>archimedean-chords</v>
       </c>
-      <c r="X18" s="2" t="str">
+      <c r="Z18" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Archimedean Chords](#archimedean-chords)</v>
       </c>
-      <c r="Y18" s="2" t="str">
+      <c r="AA18" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2815,7 +2935,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2825,77 +2945,83 @@
       <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>2</v>
       </c>
-      <c r="H19" t="str">
+      <c r="J19" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>4</v>
       </c>
-      <c r="J19" t="str">
+      <c r="L19" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>9</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>30</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>148.72</v>
       </c>
-      <c r="O19" s="2">
+      <c r="Q19" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99420071864293469</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="R19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>570</v>
       </c>
-      <c r="R19" s="2">
+      <c r="T19" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.0932868352223191</v>
       </c>
-      <c r="S19" s="2" t="str">
+      <c r="U19" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="T19" s="3">
+      <c r="V19" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.26091228070175437</v>
       </c>
-      <c r="U19" s="2">
+      <c r="W19" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.96255695187019885</v>
       </c>
-      <c r="V19" t="s">
+      <c r="X19" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="2" t="str">
+      <c r="Y19" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>octagram-spiral</v>
       </c>
-      <c r="X19" s="2" t="str">
+      <c r="Z19" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Octagram Spiral](#octagram-spiral)</v>
       </c>
-      <c r="Y19" s="2" t="str">
+      <c r="AA19" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -2918,7 +3044,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2928,77 +3054,83 @@
       <c r="C20" t="s">
         <v>82</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>2</v>
       </c>
-      <c r="H20" t="str">
+      <c r="J20" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>2</v>
       </c>
-      <c r="J20" t="str">
+      <c r="L20" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>2</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>50</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>49.39</v>
       </c>
-      <c r="O20" s="2">
+      <c r="Q20" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.33017464694576754</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="R20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>170</v>
       </c>
-      <c r="R20" s="2">
+      <c r="T20" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.32606800348735832</v>
       </c>
-      <c r="S20" s="2" t="str">
+      <c r="U20" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Extra-Low</v>
       </c>
-      <c r="T20" s="3">
+      <c r="V20" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.29052941176470587</v>
       </c>
-      <c r="U20" s="2">
+      <c r="W20" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.0718203998091715</v>
       </c>
-      <c r="V20" t="s">
+      <c r="X20" t="s">
         <v>26</v>
       </c>
-      <c r="W20" s="2" t="str">
+      <c r="Y20" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>support-cubic</v>
       </c>
-      <c r="X20" s="2" t="str">
+      <c r="Z20" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Support Cubic](#support-cubic)</v>
       </c>
-      <c r="Y20" s="2" t="str">
+      <c r="AA20" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3021,78 +3153,84 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="60" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+    <row r="21" spans="1:27" ht="120" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>2</v>
       </c>
-      <c r="H21" t="str">
+      <c r="J21" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>2</v>
       </c>
-      <c r="J21" t="str">
+      <c r="L21" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Low</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>1</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>16</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>12.33</v>
       </c>
-      <c r="O21" s="2">
+      <c r="Q21" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>8.2426673351717217E-2</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="R21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>76</v>
       </c>
-      <c r="R21" s="2">
+      <c r="T21" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.14577157802964255</v>
       </c>
-      <c r="S21" s="2" t="str">
+      <c r="U21" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Ultra-Low</v>
       </c>
-      <c r="T21" s="3">
+      <c r="V21" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.16223684210526315</v>
       </c>
-      <c r="U21" s="2">
+      <c r="W21" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.59852376361078963</v>
       </c>
-      <c r="V21" t="s">
+      <c r="X21" t="s">
         <v>25</v>
       </c>
-      <c r="W21" s="2" t="str">
+      <c r="Y21" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>lightning</v>
       </c>
-      <c r="X21" s="2" t="str">
+      <c r="Z21" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Lightning](#lightning)</v>
       </c>
-      <c r="Y21" s="2" t="str">
+      <c r="AA21" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3115,78 +3253,84 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="22" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>5</v>
       </c>
-      <c r="H22" t="str">
+      <c r="J22" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>5</v>
       </c>
-      <c r="J22" t="str">
+      <c r="L22" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>Normal-High</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>10</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>40</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>144.69999999999999</v>
       </c>
-      <c r="O22" s="2">
+      <c r="Q22" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.96732681540904142</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="R22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>640</v>
       </c>
-      <c r="R22" s="2">
+      <c r="T22" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>1.2275501307759371</v>
       </c>
-      <c r="S22" s="2" t="str">
+      <c r="U22" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-High</v>
       </c>
-      <c r="T22" s="3">
+      <c r="V22" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.22609374999999998</v>
       </c>
-      <c r="U22" s="2">
+      <c r="W22" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>0.83410451302470801</v>
       </c>
-      <c r="V22" t="s">
+      <c r="X22" t="s">
         <v>24</v>
       </c>
-      <c r="W22" s="2" t="str">
+      <c r="Y22" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>cross-hatch</v>
       </c>
-      <c r="X22" s="2" t="str">
+      <c r="Z22" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Cross Hatch](#cross-hatch)</v>
       </c>
-      <c r="Y22" s="2" t="str">
+      <c r="AA22" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3209,78 +3353,84 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+    <row r="23" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>6</v>
       </c>
-      <c r="H23" t="str">
+      <c r="J23" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[XY-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>6</v>
       </c>
-      <c r="J23" t="str">
+      <c r="L23" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[Z-N]],Rating[N],Rating[Name])</f>
         <v>High</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>8</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>1</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>148.55000000000001</v>
       </c>
-      <c r="O23" s="2">
+      <c r="Q23" s="2">
         <f>Infill[[#This Row],[g]]/(997.25*0.15)</f>
         <v>0.99306426004846671</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="R23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <f>Infill[[#This Row],[hs]]*60+Infill[[#This Row],[min]]</f>
         <v>481</v>
       </c>
-      <c r="R23" s="2">
+      <c r="T23" s="2">
         <f>Infill[[#This Row],[Total Time]]/AVERAGE(Infill[Total Time])</f>
         <v>0.92258064516129035</v>
       </c>
-      <c r="S23" s="2" t="str">
+      <c r="U23" s="2" t="str">
         <f>_xlfn.XLOOKUP(Infill[[#This Row],[t prom]],Rating[Max %],Rating[Name],,1)</f>
         <v>Normal-Low</v>
       </c>
-      <c r="T23" s="3">
+      <c r="V23" s="3">
         <f>Infill[[#This Row],[g]]/Infill[[#This Row],[Total Time]]</f>
         <v>0.30883575883575887</v>
       </c>
-      <c r="U23" s="2">
+      <c r="W23" s="2">
         <f>Infill[[#This Row],[g/t]]/AVERAGE(Infill[g/t])</f>
         <v>1.1393561309338132</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="W23" s="2" t="str">
+      <c r="Y23" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
         <v>quarter-cubic</v>
       </c>
-      <c r="X23" s="2" t="str">
+      <c r="Z23" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
         <v>[Quarter Cubic](#quarter-cubic)</v>
       </c>
-      <c r="Y23" s="2" t="str">
+      <c r="AA23" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -3305,7 +3455,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="O2:O23">
+  <conditionalFormatting sqref="Q2:Q23">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3317,7 +3467,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R23">
+  <conditionalFormatting sqref="T2:T23">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3329,7 +3479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T23">
+  <conditionalFormatting sqref="V2:V23">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3341,7 +3491,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U23">
+  <conditionalFormatting sqref="W2:W23">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Fixes, typos and Infill improvements
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB36A0C1-CA40-4C90-A458-7C2666F59840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18C77CD-4FEB-4443-8ED0-9539E823167A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
@@ -227,12 +227,6 @@
     <t>Similar to the [triangles](#triangles) pattern but offset to prevent triple overlaps at intersections. This design combines triangles and hexagons, providing excellent X-Y strength.</t>
   </si>
   <si>
-    <t>Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure.</t>
-  </si>
-  <si>
-    <t>Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions.</t>
-  </si>
-  <si>
     <t>Hexagonal pattern balancing strength and material use. Double walls in each hexagon increase material consumption.</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
 Recommended with layer anchoring to improve not perpendicular strength.</t>
   </si>
   <si>
-    <t>This infill tries to generate a printable honeycomb structure by printing squares and octagons mantaining a vertical angle high enough to mantian contact with the previous layer.</t>
-  </si>
-  <si>
     <t>Spiral pattern that fills the area with concentric arcs, creating a smooth and continuous infill. Can be filled with resin thanks to its interconnected hollow structure, which allows the resin to flow through it and cure properly.</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>Ultra-fast, ultra-low material infill. Designed for speed and efficiency, ideal for quick prints or non-structural prototypes.</t>
   </si>
   <si>
-    <t>Similar to [Gyroid](#gyroid) but with linear patterns, creating weak points at internal corners.</t>
-  </si>
-  <si>
     <t>[Cubic](#cubic) pattern with extra internal divisions, improving X-Y strength.</t>
   </si>
   <si>
@@ -277,12 +265,6 @@
   </si>
   <si>
     <t>Ultra-High</t>
-  </si>
-  <si>
-    <t>Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve interlayer point of contact and reduce the risk of delamination.</t>
-  </si>
-  <si>
-    <t>Low-strength pattern with good flexibility. Angle 1 and angle 2 TBD.</t>
   </si>
   <si>
     <t>Esthetic pattern with low strength and high print time.</t>
@@ -325,24 +307,9 @@
     <t>Zig Zag</t>
   </si>
   <si>
-    <t>Coss Zag</t>
-  </si>
-  <si>
     <t>Locked Zag</t>
   </si>
   <si>
-    <t>Similar to [rectilinear](#rectilinear) with consistent pattern between layers. Allows you to add a Symmetric infil Y axis for models with two symmetric parts.</t>
-  </si>
-  <si>
-    <t>Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding. Considere using new [Zig Zag](#zig-zag) infill instead.</t>
-  </si>
-  <si>
-    <t>Similar to [Zig Zag](#zig-zag) but displacing each lager with Infill shift step parammeter.</t>
-  </si>
-  <si>
-    <t>Adaptative version of [Zig Zag](#zig-zag) adding an external skin texture to interlock layers and a low material skeleton.</t>
-  </si>
-  <si>
     <t>Same as [Zig Zag](#zig-zag) but increasing near walls</t>
   </si>
   <si>
@@ -350,6 +317,40 @@
   </si>
   <si>
     <t>Pattern</t>
+  </si>
+  <si>
+    <t>Cross Zag</t>
+  </si>
+  <si>
+    <t>Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding. Consider using new [Zig Zag](#zig-zag) infill instead.</t>
+  </si>
+  <si>
+    <t>Low-strength pattern with good flexibility. You can adjust **Angle 1** and **Angle 2** to optimize the infill for your specific model. Each angle adjusts the plane of each layer generated by the pattern. 0° is vertical.</t>
+  </si>
+  <si>
+    <t>Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure. This pattern may require more time to slice because of all the points needed to generate each curve. If your model has complex geometry, consider using a simpler infill pattern like [TPMS-D](#tpms-d) or [Cross Hatch](#cross-hatch).</t>
+  </si>
+  <si>
+    <t>Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.</t>
+  </si>
+  <si>
+    <t>Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve the point of contact between layers and reduce the risk of delamination.</t>
+  </si>
+  <si>
+    <t>This infill tries to generate a printable honeycomb structure by printing squares and octagons maintaining a vertical angle high enough to maintain contact with the previous layer.</t>
+  </si>
+  <si>
+    <t>Similar to [Gyroid](#gyroid) but with linear patterns, creating weak points at internal corners.
+Easier to slice but consider using [TPMS-D](#tpms-d) or [Gyroid](#gyroid) for better strength and flexibility.</t>
+  </si>
+  <si>
+    <t>Similar to [rectilinear](#rectilinear) with consistent pattern between layers. Allows you to add a Symmetric infill Y axis for models with two symmetric parts.</t>
+  </si>
+  <si>
+    <t>Similar to [Zig Zag](#zig-zag) but displacing each layer with Infill shift step parameter.</t>
+  </si>
+  <si>
+    <t>Adaptive version of [Zig Zag](#zig-zag) adding an external skin texture to interlock layers and a low material skeleton.</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,10 +1065,10 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1100,7 +1101,7 @@
         <v>32</v>
       </c>
       <c r="Q1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
@@ -1109,28 +1110,28 @@
         <v>49</v>
       </c>
       <c r="T1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="U1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="V1" t="s">
         <v>50</v>
       </c>
       <c r="W1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="X1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Y1" t="s">
         <v>43</v>
       </c>
       <c r="Z1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="AA1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="120" x14ac:dyDescent="0.25">
@@ -1167,7 +1168,7 @@
         <v>Normal</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N2">
         <v>8</v>
@@ -1258,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -1275,7 +1276,7 @@
         <v>Low</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N3">
         <v>8</v>
@@ -1338,7 +1339,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Rectilinear
-Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding. Considere using new [Zig Zag](#zig-zag) infill instead.
+Parallel lines spaced according to infill density. Each layer is printed perpendicular to the previous, resulting in low vertical bonding. Consider using new [Zig Zag](#zig-zag) infill instead.
 - **Horizontal Strength (X-Y):** Normal-Low
 - **Vertical Strength (Z):** Low
 - **Density Calculation:**  % of  total infill volume
@@ -1383,7 +1384,7 @@
         <v>High</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N4">
         <v>8</v>
@@ -1457,7 +1458,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -1491,7 +1492,7 @@
         <v>Low</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N5">
         <v>8</v>
@@ -1554,7 +1555,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Lattice
-Low-strength pattern with good flexibility. Angle 1 and angle 2 TBD.
+Low-strength pattern with good flexibility. You can adjust **Angle 1** and **Angle 2** to optimize the infill for your specific model. Each angle adjusts the plane of each layer generated by the pattern. 0° is vertical.
 - **Horizontal Strength (X-Y):** Normal-Low
 - **Vertical Strength (Z):** Low
 - **Density Calculation:**  % of  total infill volume
@@ -1599,7 +1600,7 @@
         <v>Low</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N6">
         <v>7</v>
@@ -1707,7 +1708,7 @@
         <v>High</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N7">
         <v>7</v>
@@ -1815,7 +1816,7 @@
         <v>Normal</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N8">
         <v>7</v>
@@ -1923,7 +1924,7 @@
         <v>Normal-High</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N9">
         <v>7</v>
@@ -1997,7 +1998,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="360" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>9</v>
       </c>
@@ -2008,7 +2009,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="I10">
         <v>6</v>
@@ -2025,7 +2026,7 @@
         <v>High</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N10">
         <v>10</v>
@@ -2088,7 +2089,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Gyroid
-Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure.
+Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure. This pattern may require more time to slice because of all the points needed to generate each curve. If your model has complex geometry, consider using a simpler infill pattern like [TPMS-D](#tpms-d) or [Cross Hatch](#cross-hatch).
 - **Horizontal Strength (X-Y):** High
 - **Vertical Strength (Z):** High
 - **Density Calculation:**  % of  total infill volume
@@ -2099,12 +2100,12 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="255" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -2119,7 +2120,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -2136,7 +2137,7 @@
         <v>High</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N11">
         <v>11</v>
@@ -2199,7 +2200,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### TPMS-D
-Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions.
+Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.
 - **Horizontal Strength (X-Y):** High
 - **Vertical Strength (Z):** High
 - **Density Calculation:**  % of  total infill volume
@@ -2218,7 +2219,7 @@
         <v>0.15</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E12">
         <v>11</v>
@@ -2230,7 +2231,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -2247,7 +2248,7 @@
         <v>High</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N12">
         <v>17</v>
@@ -2329,7 +2330,7 @@
         <v>0.4</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -2341,7 +2342,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I13">
         <v>5</v>
@@ -2358,7 +2359,7 @@
         <v>Normal-High</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N13">
         <v>5</v>
@@ -2452,7 +2453,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I14">
         <v>3</v>
@@ -2469,7 +2470,7 @@
         <v>Normal</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N14">
         <v>8</v>
@@ -2544,7 +2545,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="300" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="315" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2561,10 +2562,10 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -2581,7 +2582,7 @@
         <v>Normal-Low</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N15">
         <v>8</v>
@@ -2644,7 +2645,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 2D Honeycomb
-Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve interlayer point of contact and reduce the risk of delamination.
+Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve the point of contact between layers and reduce the risk of delamination.
 - **Horizontal Strength (X-Y):** Normal-Low
 - **Vertical Strength (Z):** Normal-Low
 - **Density Calculation:**  % of  total infill volume
@@ -2675,7 +2676,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -2755,7 +2756,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### 3D Honeycomb
-This infill tries to generate a printable honeycomb structure by printing squares and octagons mantaining a vertical angle high enough to mantian contact with the previous layer.
+This infill tries to generate a printable honeycomb structure by printing squares and octagons maintaining a vertical angle high enough to maintain contact with the previous layer.
 - **Horizontal Strength (X-Y):** Normal-High
 - **Vertical Strength (Z):** Normal-High
 - **Density Calculation:** Unknown
@@ -2786,7 +2787,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -2803,7 +2804,7 @@
         <v>Normal</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N17">
         <v>13</v>
@@ -2898,7 +2899,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -2915,7 +2916,7 @@
         <v>Normal</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N18">
         <v>7</v>
@@ -2997,7 +2998,7 @@
         <v>1.85</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E19">
         <v>18</v>
@@ -3009,7 +3010,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -3026,7 +3027,7 @@
         <v>Normal</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N19">
         <v>9</v>
@@ -3108,7 +3109,7 @@
         <v>9.99</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E20">
         <v>19</v>
@@ -3120,7 +3121,7 @@
         <v>18</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -3137,7 +3138,7 @@
         <v>Low</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -3222,7 +3223,7 @@
         <v>19</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -3239,7 +3240,7 @@
         <v>Low</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -3313,7 +3314,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="180" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>21</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="I22">
         <v>5</v>
@@ -3341,7 +3342,7 @@
         <v>Normal-High</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N22">
         <v>10</v>
@@ -3405,6 +3406,7 @@
 "</f>
         <v xml:space="preserve">### Cross Hatch
 Similar to [Gyroid](#gyroid) but with linear patterns, creating weak points at internal corners.
+Easier to slice but consider using [TPMS-D](#tpms-d) or [Gyroid](#gyroid) for better strength and flexibility.
 - **Horizontal Strength (X-Y):** Normal-High
 - **Vertical Strength (Z):** Normal-High
 - **Density Calculation:**  % of  total infill volume
@@ -3426,7 +3428,7 @@
         <v>44</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I23">
         <v>6</v>
@@ -3443,7 +3445,7 @@
         <v>High</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N23">
         <v>8</v>
@@ -3525,10 +3527,10 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I24">
         <v>3</v>
@@ -3545,7 +3547,7 @@
         <v>Low</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N24">
         <v>8</v>
@@ -3608,7 +3610,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Zig Zag
-Similar to [rectilinear](#rectilinear) with consistent pattern between layers. Allows you to add a Symmetric infil Y axis for models with two symmetric parts.
+Similar to [rectilinear](#rectilinear) with consistent pattern between layers. Allows you to add a Symmetric infill Y axis for models with two symmetric parts.
 - **Horizontal Strength (X-Y):** Normal-Low
 - **Vertical Strength (Z):** Low
 - **Density Calculation:**  % of  total infill volume
@@ -3627,10 +3629,10 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I25">
         <v>4</v>
@@ -3647,7 +3649,7 @@
         <v>Low</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N25">
         <v>8</v>
@@ -3692,11 +3694,11 @@
       </c>
       <c r="Y25" s="2" t="str">
         <f>SUBSTITUTE(LOWER(Infill[[#This Row],[Infill]])," ","-")</f>
-        <v>coss-zag</v>
+        <v>cross-zag</v>
       </c>
       <c r="Z25" s="2" t="str">
         <f>"["&amp;Infill[[#This Row],[Infill]]&amp;"](#"&amp;Infill[[#This Row],[image]]&amp;")"</f>
-        <v>[Coss Zag](#coss-zag)</v>
+        <v>[Cross Zag](#cross-zag)</v>
       </c>
       <c r="AA25" s="2" t="str">
         <f>"### "&amp;Infill[[#This Row],[Infill]]&amp;"
@@ -3709,15 +3711,15 @@
 - **Material/Time (Higher better):** "&amp;Infill[[#This Row],[Material/Time]]&amp;"
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
-        <v xml:space="preserve">### Coss Zag
-Similar to [Zig Zag](#zig-zag) but displacing each lager with Infill shift step parammeter.
+        <v xml:space="preserve">### Cross Zag
+Similar to [Zig Zag](#zig-zag) but displacing each layer with Infill shift step parameter.
 - **Horizontal Strength (X-Y):** Normal
 - **Vertical Strength (Z):** Low
 - **Density Calculation:**  % of  total infill volume
 - **Material Usage:** Normal
 - **Print Time:** Normal
 - **Material/Time (Higher better):** Normal
-![infill-top-coss-zag](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-coss-zag.png?raw=true)
+![infill-top-cross-zag](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-cross-zag.png?raw=true)
 </v>
       </c>
     </row>
@@ -3729,10 +3731,10 @@
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -3749,7 +3751,7 @@
         <v>Normal-Low</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="N26">
         <v>15</v>
@@ -3812,7 +3814,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### Locked Zag
-Adaptative version of [Zig Zag](#zig-zag) adding an external skin texture to interlock layers and a low material skeleton.
+Adaptive version of [Zig Zag](#zig-zag) adding an external skin texture to interlock layers and a low material skeleton.
 - **Horizontal Strength (X-Y):** Normal-Low
 - **Vertical Strength (Z):** Normal-Low
 - **Density Calculation:** Same as [Zig Zag](#zig-zag) but increasing near walls

</xml_diff>

<commit_message>
Clarify TPMS-D infill description
Updated the TPMS-D infill section to specify that it refers to the Schwarz Diamond surface, improving clarity for users. Also updated the infill calculator spreadsheet.

Co-Authored-By: Rodrigo <162915171+RF47@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18C77CD-4FEB-4443-8ED0-9539E823167A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FA49AC-1CB2-4B38-920C-5F200A994927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t>Mathematical, isotropic surface providing equal strength in all directions. Excellent for strong, flexible prints and resin filling due to its interconnected structure. This pattern may require more time to slice because of all the points needed to generate each curve. If your model has complex geometry, consider using a simpler infill pattern like [TPMS-D](#tpms-d) or [Cross Hatch](#cross-hatch).</t>
   </si>
   <si>
-    <t>Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.</t>
-  </si>
-  <si>
     <t>Vertical Honeycomb pattern. Acceptable torsional stiffness. Developed for low densities structures like wings. Improve over [2D Lattice](#2d-lattice) offers same performance with lower densities.This infill includes a Overhang angle parameter to improve the point of contact between layers and reduce the risk of delamination.</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>Adaptive version of [Zig Zag](#zig-zag) adding an external skin texture to interlock layers and a low material skeleton.</t>
+  </si>
+  <si>
+    <t>Triply Periodic Minimal Surface (Schwarz Diamond). Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2100,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="255" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="270" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -2200,7 +2200,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[image]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[image]]&amp;".png?raw=true)
 "</f>
         <v xml:space="preserve">### TPMS-D
-Triply Periodic Minimal Surface - D. Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.
+Triply Periodic Minimal Surface (Schwarz Diamond). Hybrid between [Cross Hatch](#cross-hatch) and [Gyroid](#gyroid), combining rigidity and smooth transitions. Isotropic and strong in all directions. This geometry is faster to slice than Gyroid, but slower than Cross Hatch.
 - **Horizontal Strength (X-Y):** High
 - **Vertical Strength (Z):** High
 - **Density Calculation:**  % of  total infill volume
@@ -2565,7 +2565,7 @@
         <v>71</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -2676,7 +2676,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -3325,7 +3325,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I22">
         <v>5</v>
@@ -3530,7 +3530,7 @@
         <v>88</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I24">
         <v>3</v>
@@ -3632,7 +3632,7 @@
         <v>93</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25">
         <v>4</v>
@@ -3734,7 +3734,7 @@
         <v>89</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I26">
         <v>3</v>

</xml_diff>

<commit_message>
Renaming compatibility fix + Rename Wiki
Co-Authored-By: SoftFever <softfeverever@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290C59A5-7D81-4F43-8A31-44709A915841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932860C-A094-4F2F-8095-75715BF224A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -440,9 +440,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>zig-zag</t>
-  </si>
-  <si>
     <t>concentric</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>[Rectilinear](#rectilinear) in a uniform direction for a smoother visual surface.</t>
+  </si>
+  <si>
+    <t>rectilinear</t>
   </si>
 </sst>
 </file>
@@ -1398,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,28 +1452,28 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
         <v>163</v>
-      </c>
-      <c r="H1" t="s">
-        <v>164</v>
       </c>
       <c r="I1" t="s">
         <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K1" t="s">
         <v>131</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M1" t="s">
         <v>41</v>
@@ -1530,10 +1530,10 @@
         <v>42</v>
       </c>
       <c r="AE1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AF1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG1" t="s">
         <v>89</v>
@@ -1542,13 +1542,13 @@
         <v>84</v>
       </c>
       <c r="AI1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AJ1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK1" t="s">
         <v>165</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="105" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>91</v>
@@ -1648,7 +1648,7 @@
         <v>rectilinear</v>
       </c>
       <c r="AE2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AF2" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -1682,11 +1682,11 @@
       </c>
       <c r="AI2" t="str">
         <f>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]])," { """&amp;Infill[[#This Row],[infill]]&amp;""", "&amp;Infill[[#This Row],[ip]]&amp;" },","")</f>
-        <v xml:space="preserve"> { "zig-zag", ipRectilinear },</v>
+        <v xml:space="preserve"> { "rectilinear", ipRectilinear },</v>
       </c>
       <c r="AJ2" t="str">
         <f>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]]),"def-&gt;enum_values.push_back("""&amp;Infill[[#This Row],[infill]]&amp;""");","")</f>
-        <v>def-&gt;enum_values.push_back("zig-zag");</v>
+        <v>def-&gt;enum_values.push_back("rectilinear");</v>
       </c>
       <c r="AK2" t="str">
         <f>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]]),"def-&gt;enum_labels.push_back(L("""&amp;Infill[[#This Row],[name]]&amp;"""));","")</f>
@@ -1722,7 +1722,7 @@
         <v>115</v>
       </c>
       <c r="L3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>64</v>
@@ -1790,7 +1790,7 @@
         <v>aligned-rectilinear</v>
       </c>
       <c r="AE3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AF3" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -1865,7 +1865,7 @@
         <v>127</v>
       </c>
       <c r="L4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>97</v>
@@ -1933,7 +1933,7 @@
         <v>zig-zag</v>
       </c>
       <c r="AE4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF4" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2007,7 +2007,7 @@
         <v>128</v>
       </c>
       <c r="L5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>98</v>
@@ -2075,7 +2075,7 @@
         <v>cross-zag</v>
       </c>
       <c r="AE5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF5" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2149,7 +2149,7 @@
         <v>129</v>
       </c>
       <c r="L6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>99</v>
@@ -2217,7 +2217,7 @@
         <v>locked-zag</v>
       </c>
       <c r="AE6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF6" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2291,7 +2291,7 @@
         <v>105</v>
       </c>
       <c r="L7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>58</v>
@@ -2359,7 +2359,7 @@
         <v>line</v>
       </c>
       <c r="AE7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AF7" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2427,13 +2427,13 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K8" t="s">
         <v>103</v>
       </c>
       <c r="L8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>57</v>
@@ -2501,7 +2501,7 @@
         <v>grid</v>
       </c>
       <c r="AE8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AF8" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2566,19 +2566,19 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K9" t="s">
         <v>113</v>
       </c>
       <c r="L9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N9">
         <v>3</v>
@@ -2637,7 +2637,7 @@
         <v>monotonic</v>
       </c>
       <c r="AE9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AF9" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2687,19 +2687,19 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K10" t="s">
         <v>114</v>
       </c>
       <c r="L10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N10">
         <v>3</v>
@@ -2758,7 +2758,7 @@
         <v>monotonic-line</v>
       </c>
       <c r="AE10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AF10" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2820,13 +2820,13 @@
         <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K11" t="s">
         <v>107</v>
       </c>
       <c r="L11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>60</v>
@@ -2894,7 +2894,7 @@
         <v>triangles</v>
       </c>
       <c r="AE11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF11" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -2965,13 +2965,13 @@
         <v>7</v>
       </c>
       <c r="J12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K12" t="s">
         <v>108</v>
       </c>
       <c r="L12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>61</v>
@@ -3039,7 +3039,7 @@
         <v>tri-hexagon</v>
       </c>
       <c r="AE12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF12" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3116,7 +3116,7 @@
         <v>106</v>
       </c>
       <c r="L13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>59</v>
@@ -3184,7 +3184,7 @@
         <v>cubic</v>
       </c>
       <c r="AE13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AF13" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3261,7 +3261,7 @@
         <v>112</v>
       </c>
       <c r="L14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>63</v>
@@ -3329,7 +3329,7 @@
         <v>adaptive-cubic</v>
       </c>
       <c r="AE14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF14" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3406,7 +3406,7 @@
         <v>126</v>
       </c>
       <c r="L15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>68</v>
@@ -3474,7 +3474,7 @@
         <v>quarter-cubic</v>
       </c>
       <c r="AE15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF15" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3545,13 +3545,13 @@
         <v>17</v>
       </c>
       <c r="J16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K16" t="s">
         <v>121</v>
       </c>
       <c r="L16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>66</v>
@@ -3619,7 +3619,7 @@
         <v>support-cubic</v>
       </c>
       <c r="AE16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AF16" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3690,13 +3690,13 @@
         <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K17" t="s">
         <v>124</v>
       </c>
       <c r="L17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>67</v>
@@ -3764,7 +3764,7 @@
         <v>lightning</v>
       </c>
       <c r="AE17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AF17" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3841,7 +3841,7 @@
         <v>111</v>
       </c>
       <c r="L18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>62</v>
@@ -3909,7 +3909,7 @@
         <v>honeycomb</v>
       </c>
       <c r="AE18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF18" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -3986,7 +3986,7 @@
         <v>117</v>
       </c>
       <c r="L19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>95</v>
@@ -4054,7 +4054,7 @@
         <v>3d-honeycomb</v>
       </c>
       <c r="AE19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AF19" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4131,7 +4131,7 @@
         <v>116</v>
       </c>
       <c r="L20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M20" s="8" t="s">
         <v>94</v>
@@ -4199,7 +4199,7 @@
         <v>2d-honeycomb</v>
       </c>
       <c r="AE20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AF20" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4261,13 +4261,13 @@
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K21" t="s">
         <v>104</v>
       </c>
       <c r="L21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>92</v>
@@ -4335,7 +4335,7 @@
         <v>2d-lattice</v>
       </c>
       <c r="AE21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF21" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4397,13 +4397,13 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K22" t="s">
         <v>125</v>
       </c>
       <c r="L22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M22" s="6" t="s">
         <v>96</v>
@@ -4471,7 +4471,7 @@
         <v>cross-hatch</v>
       </c>
       <c r="AE22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AF22" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4534,13 +4534,13 @@
         <v>9</v>
       </c>
       <c r="J23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K23" t="s">
         <v>110</v>
       </c>
       <c r="L23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>100</v>
@@ -4608,7 +4608,7 @@
         <v>tpms-d</v>
       </c>
       <c r="AE23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AF23" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4670,13 +4670,13 @@
         <v>8</v>
       </c>
       <c r="J24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K24" t="s">
         <v>109</v>
       </c>
       <c r="L24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>93</v>
@@ -4744,7 +4744,7 @@
         <v>gyroid</v>
       </c>
       <c r="AE24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF24" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4806,13 +4806,13 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K25" t="s">
         <v>101</v>
       </c>
       <c r="L25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>56</v>
@@ -4880,7 +4880,7 @@
         <v>concentric</v>
       </c>
       <c r="AE25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AF25" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -4942,13 +4942,13 @@
         <v>14</v>
       </c>
       <c r="J26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K26" t="s">
         <v>118</v>
       </c>
       <c r="L26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>76</v>
@@ -5016,7 +5016,7 @@
         <v>hilbert-curve</v>
       </c>
       <c r="AE26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AF26" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -5079,13 +5079,13 @@
         <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K27" t="s">
         <v>119</v>
       </c>
       <c r="L27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>65</v>
@@ -5153,7 +5153,7 @@
         <v>archimedean-chords</v>
       </c>
       <c r="AE27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF27" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>
@@ -5215,13 +5215,13 @@
         <v>16</v>
       </c>
       <c r="J28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K28" t="s">
         <v>120</v>
       </c>
       <c r="L28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>75</v>
@@ -5289,7 +5289,7 @@
         <v>octagram-spiral</v>
       </c>
       <c r="AE28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF28" t="str">
         <f>"!["&amp;Infill[[#This Row],[SVG]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/resources/images/"&amp;Infill[[#This Row],[SVG]]&amp;".svg?raw=true)"</f>

</xml_diff>

<commit_message>
Wiki Update 12 - Others (#10452)
* Update others_settings_brim.md

* Improved brim

* brim wiki

* Update others_settings_brim.md

* Skirt

* Icons to settings sections

* Create Built-in-placeholders-variables.md

* Update others_settings_g_code_output.md

* Update others_settings_notes.md

* Update others_settings_post_processing_scripts.md

* special mode

* Fuzzy skin

* Image fix

* PA update

* Update pressure-advance-calib.md

* Phishing report link in README

* pa wiki link

* Esthetic -> Aesthetic
</commit_message>
<xml_diff>
--- a/doc/print_settings/strength/infill_desc_calculator.xlsx
+++ b/doc/print_settings/strength/infill_desc_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repos\OrcaSlicer\doc\print_settings\strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9342C-2BC8-4E65-A1F6-5FE50430102E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0746496-878A-4475-889F-BAAA76C0EE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7BCEEB8-8D62-4686-9FA1-C052039D2FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -255,13 +255,6 @@
     <t>Ultra-High</t>
   </si>
   <si>
-    <t>Esthetic pattern with low strength and high print time.</t>
-  </si>
-  <si>
-    <t>Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its Esthetic appeal and ability to fill space efficiently.
-Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for Esthetic purposes.</t>
-  </si>
-  <si>
     <t>Max %</t>
   </si>
   <si>
@@ -530,9 +523,6 @@
     <t>TPMS</t>
   </si>
   <si>
-    <t>Esthetic</t>
-  </si>
-  <si>
     <t>Support</t>
   </si>
   <si>
@@ -621,6 +611,16 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Aesthetic</t>
+  </si>
+  <si>
+    <t>Aesthetic pattern with low strength and high print time.</t>
+  </si>
+  <si>
+    <t>Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its aesthetic appeal and ability to fill space efficiently.
+Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for aesthetic purposes.</t>
   </si>
 </sst>
 </file>
@@ -698,10 +698,6 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -736,6 +732,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1018,12 +1018,12 @@
     <tableColumn id="21" xr3:uid="{75AA760A-15C0-4692-B168-BF74BE6D50F6}" name="Pattern" dataDxfId="13" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>"["&amp;Infill[[#This Row],[name]]&amp;"](#"&amp;Infill[[#This Row],[nameMD]]&amp;")"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{D12C345A-0415-4208-969C-FE76BD14B76A}" name="Applies to" dataDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="31" xr3:uid="{D12C345A-0415-4208-969C-FE76BD14B76A}" name="Applies to" dataDxfId="12" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Infill[[#This Row],[Is Infill]],"  - **[Sparse Infill](strength_settings_infill#sparse-infill-density)**",)&amp;IF(Infill[[#This Row],[Is Surface]],"  - **[Solid Infill](strength_settings_infill#internal-solid-infill)**",)&amp;IF(Infill[[#This Row],[Is Surface]],"
   - **[Surface](strength_settings_top_bottom_shells)**",)&amp;IF(Infill[[#This Row],[Is Ironing]],"
   - **[Ironing](quality_settings_ironing)**",)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="MD" dataDxfId="12" dataCellStyle="Porcentaje">
+    <tableColumn id="14" xr3:uid="{AE92B56B-1C4F-4A43-BC18-AFFF1480255E}" name="MD" dataDxfId="11" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]],Infill[[#This Row],[Is Ironing]]),"## "&amp;Infill[[#This Row],[name]]&amp;"
 "&amp;Infill[[#This Row],[Desc]]&amp;"
 - **Horizontal Strength (X-Y):** "&amp;Infill[[#This Row],[X-Y Strength]]&amp;"
@@ -1037,13 +1037,13 @@
 ![infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;".png?raw=true)
 ","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{B5B3DE03-E8E0-4448-BA81-E5B849AC0415}" name="s_keys_map" dataDxfId="11" dataCellStyle="Porcentaje">
+    <tableColumn id="26" xr3:uid="{B5B3DE03-E8E0-4448-BA81-E5B849AC0415}" name="s_keys_map" dataDxfId="10" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]])," { """&amp;Infill[[#This Row],[infill]]&amp;""", "&amp;Infill[[#This Row],[ip]]&amp;" },","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{DF1D46A6-663C-4993-9678-9483ECBDC09A}" name="Enum Pattern" dataDxfId="10" dataCellStyle="Porcentaje">
+    <tableColumn id="30" xr3:uid="{DF1D46A6-663C-4993-9678-9483ECBDC09A}" name="Enum Pattern" dataDxfId="9" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]]),"def-&gt;enum_values.push_back("""&amp;Infill[[#This Row],[infill]]&amp;""");","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{A375012B-C9F3-4FDF-8EA3-593D97EDEB2B}" name="Enum Pattern Names" dataDxfId="9" dataCellStyle="Porcentaje">
+    <tableColumn id="29" xr3:uid="{A375012B-C9F3-4FDF-8EA3-593D97EDEB2B}" name="Enum Pattern Names" dataDxfId="8" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(OR(Infill[[#This Row],[Is Infill]],Infill[[#This Row],[Is Surface]]),"def-&gt;enum_labels.push_back(L("""&amp;Infill[[#This Row],[name]]&amp;"""));","")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1067,7 +1067,7 @@
   <autoFilter ref="A16:C25" xr:uid="{8371D3BF-96D7-48EB-82A0-8021F9AA952E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1D00CA6A-CEDD-45A1-8BA8-6DB7769D516C}" name="N"/>
-    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="8" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{3AC9B406-037B-4FD3-80D6-86F4D94EDB36}" name="Max %" dataDxfId="7" dataCellStyle="Porcentaje"/>
     <tableColumn id="3" xr3:uid="{18E14714-6899-4575-90B8-4F97863AF141}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1078,25 +1078,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F85400E8-93F1-42C5-93F9-13851BAE5398}" name="Tabla4" displayName="Tabla4" ref="AN1:AT32" totalsRowShown="0">
   <autoFilter ref="AN1:AT32" xr:uid="{F85400E8-93F1-42C5-93F9-13851BAE5398}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{184C8A2D-5FE4-4972-8525-02DD0ED763F3}" name="-" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{184C8A2D-5FE4-4972-8525-02DD0ED763F3}" name="-" dataDxfId="6">
       <calculatedColumnFormula>Infill[[#This Row],[SVG Link]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{14A2CB57-4B88-4948-ABB5-B4E1F3AB50EF}" name="Pattern" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{14A2CB57-4B88-4948-ABB5-B4E1F3AB50EF}" name="Pattern" dataDxfId="5">
       <calculatedColumnFormula>Infill[[#This Row],[Pattern]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7FB40202-1341-4B88-81D2-89C268F45D4D}" name="Applies to" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{7FB40202-1341-4B88-81D2-89C268F45D4D}" name="Applies to" dataDxfId="4">
       <calculatedColumnFormula>Infill[[#This Row],[Applies to]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F83791FA-52BD-4574-8359-2DC84F1575E3}" name="X-Y Strength" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{F83791FA-52BD-4574-8359-2DC84F1575E3}" name="X-Y Strength" dataDxfId="3">
       <calculatedColumnFormula>Infill[[#This Row],[X-Y Strength]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A30810A1-1E95-4BAA-97B8-93C571CB8CF0}" name="Z Strength" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{A30810A1-1E95-4BAA-97B8-93C571CB8CF0}" name="Z Strength" dataDxfId="2">
       <calculatedColumnFormula>Infill[[#This Row],[Z Strength]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{630ACA64-21F3-4422-B317-D820E5C1F820}" name="Material Usage" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{630ACA64-21F3-4422-B317-D820E5C1F820}" name="Material Usage" dataDxfId="1">
       <calculatedColumnFormula>Infill[[#This Row],[Material/Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5F0A6FFD-7381-42EE-8794-FC0492BBA85C}" name="Print Time" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{5F0A6FFD-7381-42EE-8794-FC0492BBA85C}" name="Print Time" dataDxfId="0">
       <calculatedColumnFormula>Infill[[#This Row],[Print Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1423,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F62B1C-B5D3-443B-88E3-A492D48347EC}">
   <dimension ref="A1:AT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,28 +1484,28 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M1" t="s">
         <v>40</v>
@@ -1535,7 +1535,7 @@
         <v>30</v>
       </c>
       <c r="V1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W1" t="s">
         <v>20</v>
@@ -1544,55 +1544,55 @@
         <v>46</v>
       </c>
       <c r="Y1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA1" t="s">
         <v>47</v>
       </c>
       <c r="AB1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC1" t="s">
         <v>67</v>
       </c>
       <c r="AD1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AE1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AF1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AG1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AH1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AI1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AJ1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AK1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AL1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AO1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AP1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AQ1" t="s">
         <v>27</v>
@@ -1604,7 +1604,7 @@
         <v>20</v>
       </c>
       <c r="AT1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:46" ht="314.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1627,19 +1627,19 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -1656,7 +1656,7 @@
         <v>Normal</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S2">
         <v>7</v>
@@ -1811,19 +1811,19 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -1840,7 +1840,7 @@
         <v>Normal</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S3">
         <v>9</v>
@@ -2001,13 +2001,13 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N4">
         <v>3</v>
@@ -2024,7 +2024,7 @@
         <v>Low</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S4">
         <v>8</v>
@@ -2162,7 +2162,7 @@
         <v>Normal-Low</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="270" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2188,10 +2188,10 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>62</v>
@@ -2211,7 +2211,7 @@
         <v>Normal</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S5">
         <v>8</v>
@@ -2367,19 +2367,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N6">
         <v>3</v>
@@ -2396,7 +2396,7 @@
         <v>Low</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S6">
         <v>8</v>
@@ -2548,19 +2548,19 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -2577,7 +2577,7 @@
         <v>Low</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S7">
         <v>8</v>
@@ -2729,19 +2729,19 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -2758,7 +2758,7 @@
         <v>Normal-Low</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S8">
         <v>15</v>
@@ -2916,10 +2916,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>56</v>
@@ -2939,7 +2939,7 @@
         <v>Low</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S9">
         <v>7</v>
@@ -3073,10 +3073,10 @@
     </row>
     <row r="10" spans="1:46" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -3094,13 +3094,13 @@
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>55</v>
@@ -3120,7 +3120,7 @@
         <v>High</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S10">
         <v>8</v>
@@ -3254,10 +3254,10 @@
     </row>
     <row r="11" spans="1:46" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -3275,13 +3275,13 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>58</v>
@@ -3301,7 +3301,7 @@
         <v>Normal</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S11">
         <v>7</v>
@@ -3435,10 +3435,10 @@
     </row>
     <row r="12" spans="1:46" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -3456,13 +3456,13 @@
         <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>59</v>
@@ -3482,7 +3482,7 @@
         <v>Normal-High</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S12">
         <v>7</v>
@@ -3634,10 +3634,10 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>57</v>
@@ -3657,7 +3657,7 @@
         <v>High</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S13">
         <v>7</v>
@@ -3809,10 +3809,10 @@
         <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>61</v>
@@ -3832,7 +3832,7 @@
         <v>Normal-High</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S14">
         <v>5</v>
@@ -3984,10 +3984,10 @@
         <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>66</v>
@@ -4007,7 +4007,7 @@
         <v>High</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S15">
         <v>8</v>
@@ -4144,7 +4144,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
@@ -4165,13 +4165,13 @@
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>64</v>
@@ -4191,7 +4191,7 @@
         <v>Low</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S16">
         <v>2</v>
@@ -4349,13 +4349,13 @@
         <v>17</v>
       </c>
       <c r="J17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>65</v>
@@ -4375,7 +4375,7 @@
         <v>Low</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -4536,10 +4536,10 @@
         <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>60</v>
@@ -4559,7 +4559,7 @@
         <v>High</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S18">
         <v>17</v>
@@ -4720,13 +4720,13 @@
         <v>9</v>
       </c>
       <c r="K19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N19">
         <v>5</v>
@@ -4898,19 +4898,19 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J20" t="s">
         <v>9</v>
       </c>
       <c r="K20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N20">
         <v>3</v>
@@ -4927,7 +4927,7 @@
         <v>Normal-Low</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S20">
         <v>8</v>
@@ -5082,19 +5082,19 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
+        <v>185</v>
+      </c>
+      <c r="J21" t="s">
+        <v>186</v>
+      </c>
+      <c r="K21" t="s">
+        <v>182</v>
+      </c>
+      <c r="L21" t="s">
         <v>188</v>
       </c>
-      <c r="J21" t="s">
-        <v>189</v>
-      </c>
-      <c r="K21" t="s">
-        <v>185</v>
-      </c>
-      <c r="L21" t="s">
-        <v>191</v>
-      </c>
       <c r="M21" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N21">
         <v>3</v>
@@ -5111,7 +5111,7 @@
         <v>Low</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S21">
         <v>8</v>
@@ -5269,16 +5269,16 @@
         <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N22">
         <v>5</v>
@@ -5295,7 +5295,7 @@
         <v>Normal-High</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S22">
         <v>10</v>
@@ -5454,16 +5454,16 @@
         <v>8</v>
       </c>
       <c r="J23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N23">
         <v>6</v>
@@ -5480,7 +5480,7 @@
         <v>High</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S23">
         <v>11</v>
@@ -5635,19 +5635,19 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
+        <v>170</v>
+      </c>
+      <c r="J24" t="s">
+        <v>160</v>
+      </c>
+      <c r="K24" t="s">
+        <v>168</v>
+      </c>
+      <c r="L24" t="s">
+        <v>169</v>
+      </c>
+      <c r="M24" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="J24" t="s">
-        <v>162</v>
-      </c>
-      <c r="K24" t="s">
-        <v>171</v>
-      </c>
-      <c r="L24" t="s">
-        <v>172</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="N24">
         <v>5</v>
@@ -5664,7 +5664,7 @@
         <v>Normal-High</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S24">
         <v>12</v>
@@ -5822,16 +5822,16 @@
         <v>7</v>
       </c>
       <c r="J25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N25">
         <v>6</v>
@@ -5848,7 +5848,7 @@
         <v>High</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S25">
         <v>10</v>
@@ -5997,13 +5997,13 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="K26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>54</v>
@@ -6023,7 +6023,7 @@
         <v>Normal</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S26">
         <v>8</v>
@@ -6178,16 +6178,16 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="K27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -6204,7 +6204,7 @@
         <v>Normal</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S27">
         <v>13</v>
@@ -6284,8 +6284,8 @@
 ![infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;".png?raw=true)
 ","")</f>
         <v xml:space="preserve">## Hilbert Curve
-Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its Esthetic appeal and ability to fill space efficiently.
-Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for Esthetic purposes.
+Hilbert Curve is a space-filling curve that can be used to create a continuous infill pattern. It is known for its aesthetic appeal and ability to fill space efficiently.
+Print speed is very low due to the complexity of the path, which can lead to longer print times. It is not recommended for structural parts but can be used for aesthetic purposes.
 - **Horizontal Strength (X-Y):** Low
 - **Vertical Strength (Z):** Normal
 - **Density Calculation:**  % of  total infill volume
@@ -6357,13 +6357,13 @@
         <v>14</v>
       </c>
       <c r="J28" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="K28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>63</v>
@@ -6383,7 +6383,7 @@
         <v>Normal</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S28">
         <v>7</v>
@@ -6535,16 +6535,16 @@
         <v>15</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="K29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -6561,7 +6561,7 @@
         <v>Normal</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S29">
         <v>9</v>
@@ -6641,7 +6641,7 @@
 ![infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;"](https://github.com/SoftFever/OrcaSlicer/blob/main/doc/images/fill/infill-top-"&amp;Infill[[#This Row],[nameMD]]&amp;".png?raw=true)
 ","")</f>
         <v xml:space="preserve">## Octagram Spiral
-Esthetic pattern with low strength and high print time.
+Aesthetic pattern with low strength and high print time.
 - **Horizontal Strength (X-Y):** Low
 - **Vertical Strength (Z):** Normal
 - **Density Calculation:**  % of  total infill volume
@@ -6710,7 +6710,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M30" s="8"/>
       <c r="O30" t="e">
@@ -6842,7 +6842,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M31" s="8"/>
       <c r="O31" t="e">
@@ -6974,7 +6974,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M32" s="8"/>
       <c r="O32" t="e">

</xml_diff>